<commit_message>
Populated playoff data through 1980
</commit_message>
<xml_diff>
--- a/NFL_playoff_wins.xlsx
+++ b/NFL_playoff_wins.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TomCariello\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_repositories\NFL_playoff_wins_per_team_ABC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Year</t>
   </si>
@@ -104,14 +104,29 @@
     <t>Atlanta Falcons</t>
   </si>
   <si>
-    <t>Number of playoff wins to be inserted in the table</t>
+    <t>Total Games</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Wildcard implemented</t>
+  </si>
+  <si>
+    <t>Number of playoff wins per team per year</t>
+  </si>
+  <si>
+    <t>Tampa Bay Buccaneers</t>
+  </si>
+  <si>
+    <t>San Diego Chargers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,16 +149,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -151,22 +180,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1554,448 +1607,2271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z77"/>
+  <dimension ref="A1:AD77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z20" sqref="Z20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="21" width="10.140625" customWidth="1"/>
     <col min="22" max="22" width="15.5703125" customWidth="1"/>
-    <col min="23" max="23" width="10.140625" customWidth="1"/>
-    <col min="24" max="24" width="15.85546875" customWidth="1"/>
-    <col min="25" max="25" width="10.140625" customWidth="1"/>
-    <col min="26" max="26" width="14.85546875" customWidth="1"/>
+    <col min="23" max="24" width="10.140625" customWidth="1"/>
+    <col min="25" max="26" width="15.85546875" customWidth="1"/>
+    <col min="27" max="27" width="10.140625" customWidth="1"/>
+    <col min="28" max="28" width="14.85546875" customWidth="1"/>
+    <col min="30" max="30" width="21.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="AD3" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1967</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4">
+        <v>3</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="9">
+        <f>SUM(B4:AB4)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1968</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4">
+        <v>2</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4">
+        <v>1</v>
+      </c>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="9">
+        <f t="shared" ref="AC5:AC59" si="0">SUM(B5:AB5)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>1969</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4">
+        <v>1</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4">
+        <v>2</v>
+      </c>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>1970</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4">
+        <v>2</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4">
+        <v>3</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4">
+        <v>1</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>1971</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4">
+        <v>3</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>1972</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4">
+        <v>1</v>
+      </c>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4">
+        <v>2</v>
+      </c>
+      <c r="AC9" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>1973</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>2</v>
+      </c>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>1974</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4">
+        <v>1</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4">
+        <v>1</v>
+      </c>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4">
+        <v>2</v>
+      </c>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4">
+        <v>3</v>
+      </c>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="4"/>
+      <c r="AC11" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>1975</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4">
+        <v>2</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4">
+        <v>1</v>
+      </c>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4">
+        <v>3</v>
+      </c>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>1976</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4">
+        <v>3</v>
+      </c>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4">
+        <v>1</v>
+      </c>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4">
+        <v>2</v>
+      </c>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4">
+        <v>1</v>
+      </c>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>1977</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4">
+        <v>3</v>
+      </c>
+      <c r="H14" s="4">
+        <v>2</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4">
+        <v>1</v>
+      </c>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4">
+        <v>1</v>
+      </c>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>1978</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4">
+        <v>2</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4">
+        <v>1</v>
+      </c>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4">
+        <v>3</v>
+      </c>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB15" s="4"/>
+      <c r="AC15" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AD15" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>1979</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4">
+        <v>2</v>
+      </c>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4">
+        <v>1</v>
+      </c>
+      <c r="W16" s="4">
+        <v>3</v>
+      </c>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>1980</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4">
+        <v>2</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4">
+        <v>4</v>
+      </c>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4">
+        <v>2</v>
+      </c>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>1981</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="4" t="s">
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>1982</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>1983</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>1984</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>1985</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>1986</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>1987</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>1988</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>1989</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>1990</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>1991</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2"/>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>1992</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2"/>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>1993</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2"/>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>1994</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
+      <c r="Z31" s="2"/>
+      <c r="AA31" s="2"/>
+      <c r="AB31" s="2"/>
+      <c r="AC31" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>1995</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2"/>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>1996</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2"/>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>1997</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="2"/>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>1998</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="2"/>
+      <c r="AA35" s="2"/>
+      <c r="AB35" s="2"/>
+      <c r="AC35" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>1999</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36" s="2"/>
+      <c r="Z36" s="2"/>
+      <c r="AA36" s="2"/>
+      <c r="AB36" s="2"/>
+      <c r="AC36" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="2"/>
+      <c r="AA37" s="2"/>
+      <c r="AB37" s="2"/>
+      <c r="AC37" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>2001</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2"/>
+      <c r="Y38" s="2"/>
+      <c r="Z38" s="2"/>
+      <c r="AA38" s="2"/>
+      <c r="AB38" s="2"/>
+      <c r="AC38" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>2002</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+      <c r="Y39" s="2"/>
+      <c r="Z39" s="2"/>
+      <c r="AA39" s="2"/>
+      <c r="AB39" s="2"/>
+      <c r="AC39" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>2003</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2"/>
+      <c r="Y40" s="2"/>
+      <c r="Z40" s="2"/>
+      <c r="AA40" s="2"/>
+      <c r="AB40" s="2"/>
+      <c r="AC40" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>2004</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2"/>
+      <c r="Y41" s="2"/>
+      <c r="Z41" s="2"/>
+      <c r="AA41" s="2"/>
+      <c r="AB41" s="2"/>
+      <c r="AC41" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2"/>
+      <c r="Y42" s="2"/>
+      <c r="Z42" s="2"/>
+      <c r="AA42" s="2"/>
+      <c r="AB42" s="2">
         <v>1</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="X3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z3" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1967</v>
-      </c>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1968</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1969</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1970</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1971</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1972</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1973</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1974</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1975</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1976</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1977</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1978</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1980</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1981</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1982</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1983</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1984</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1985</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1986</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1987</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1988</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1989</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1990</v>
-      </c>
-      <c r="N27" s="2"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1991</v>
-      </c>
-      <c r="N28" s="2"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1992</v>
-      </c>
-      <c r="N29" s="2"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>1993</v>
-      </c>
-      <c r="N30" s="2"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>1994</v>
-      </c>
-      <c r="N31" s="2"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>1995</v>
-      </c>
-      <c r="N32" s="2"/>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1996</v>
-      </c>
-      <c r="N33" s="2"/>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>1997</v>
-      </c>
-      <c r="N34" s="2"/>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>1998</v>
-      </c>
-      <c r="N35" s="2"/>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>1999</v>
-      </c>
-      <c r="N36" s="2"/>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>2000</v>
-      </c>
-      <c r="N37" s="2"/>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>2001</v>
-      </c>
-      <c r="N38" s="2"/>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>2002</v>
-      </c>
-      <c r="N39" s="2"/>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>2003</v>
-      </c>
-      <c r="N40" s="2"/>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>2004</v>
-      </c>
-      <c r="N41" s="2"/>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>2005</v>
-      </c>
-      <c r="N42" s="2"/>
-      <c r="Z42">
+      <c r="AC42" s="9">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
         <v>2006</v>
       </c>
-      <c r="N43" s="2"/>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2"/>
+      <c r="Y43" s="2"/>
+      <c r="Z43" s="2"/>
+      <c r="AA43" s="2"/>
+      <c r="AB43" s="2"/>
+      <c r="AC43" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
         <v>2007</v>
       </c>
-      <c r="N44" s="2"/>
-      <c r="Z44">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+      <c r="X44" s="2"/>
+      <c r="Y44" s="2"/>
+      <c r="Z44" s="2"/>
+      <c r="AA44" s="2"/>
+      <c r="AB44" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="AC44" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
         <v>2008</v>
       </c>
-      <c r="N45" s="2"/>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
+      <c r="U45" s="2"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
+      <c r="X45" s="2"/>
+      <c r="Y45" s="2"/>
+      <c r="Z45" s="2"/>
+      <c r="AA45" s="2"/>
+      <c r="AB45" s="2"/>
+      <c r="AC45" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
         <v>2009</v>
       </c>
-      <c r="N46" s="2"/>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="6"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+      <c r="S46" s="2"/>
+      <c r="T46" s="2"/>
+      <c r="U46" s="2"/>
+      <c r="V46" s="2"/>
+      <c r="W46" s="2"/>
+      <c r="X46" s="2"/>
+      <c r="Y46" s="2"/>
+      <c r="Z46" s="2"/>
+      <c r="AA46" s="2"/>
+      <c r="AB46" s="2"/>
+      <c r="AC46" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
         <v>2010</v>
       </c>
-      <c r="N47" s="2"/>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="6"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
+      <c r="V47" s="2"/>
+      <c r="W47" s="2"/>
+      <c r="X47" s="2"/>
+      <c r="Y47" s="2"/>
+      <c r="Z47" s="2"/>
+      <c r="AA47" s="2"/>
+      <c r="AB47" s="2"/>
+      <c r="AC47" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
         <v>2011</v>
       </c>
-      <c r="N48" s="2"/>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="6"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+      <c r="S48" s="2"/>
+      <c r="T48" s="2"/>
+      <c r="U48" s="2"/>
+      <c r="V48" s="2"/>
+      <c r="W48" s="2"/>
+      <c r="X48" s="2"/>
+      <c r="Y48" s="2"/>
+      <c r="Z48" s="2"/>
+      <c r="AA48" s="2"/>
+      <c r="AB48" s="2"/>
+      <c r="AC48" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
         <v>2012</v>
       </c>
-      <c r="N49" s="2"/>
-      <c r="Z49">
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+      <c r="U49" s="2"/>
+      <c r="V49" s="2"/>
+      <c r="W49" s="2"/>
+      <c r="X49" s="2"/>
+      <c r="Y49" s="2"/>
+      <c r="Z49" s="2"/>
+      <c r="AA49" s="2"/>
+      <c r="AB49" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="AC49" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
         <v>2013</v>
       </c>
-      <c r="N50" s="2"/>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="6"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+      <c r="U50" s="2"/>
+      <c r="V50" s="2"/>
+      <c r="W50" s="2"/>
+      <c r="X50" s="2"/>
+      <c r="Y50" s="2"/>
+      <c r="Z50" s="2"/>
+      <c r="AA50" s="2"/>
+      <c r="AB50" s="2"/>
+      <c r="AC50" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
         <v>2014</v>
       </c>
-      <c r="N51" s="2"/>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
+      <c r="S51" s="2"/>
+      <c r="T51" s="2"/>
+      <c r="U51" s="2"/>
+      <c r="V51" s="2"/>
+      <c r="W51" s="2"/>
+      <c r="X51" s="2"/>
+      <c r="Y51" s="2"/>
+      <c r="Z51" s="2"/>
+      <c r="AA51" s="2"/>
+      <c r="AB51" s="2"/>
+      <c r="AC51" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
         <v>2015</v>
       </c>
-      <c r="Z52">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+      <c r="S52" s="2"/>
+      <c r="T52" s="2"/>
+      <c r="U52" s="2"/>
+      <c r="V52" s="2"/>
+      <c r="W52" s="2"/>
+      <c r="X52" s="2"/>
+      <c r="Y52" s="2"/>
+      <c r="Z52" s="2"/>
+      <c r="AA52" s="2"/>
+      <c r="AB52" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="AC52" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
         <v>2016</v>
       </c>
-      <c r="N53" s="1"/>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="2"/>
+      <c r="S53" s="2"/>
+      <c r="T53" s="2"/>
+      <c r="U53" s="2"/>
+      <c r="V53" s="2"/>
+      <c r="W53" s="2"/>
+      <c r="X53" s="2"/>
+      <c r="Y53" s="2"/>
+      <c r="Z53" s="2"/>
+      <c r="AA53" s="2"/>
+      <c r="AB53" s="2"/>
+      <c r="AC53" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
         <v>2017</v>
       </c>
-      <c r="N54" s="1"/>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="2"/>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="2"/>
+      <c r="S54" s="2"/>
+      <c r="T54" s="2"/>
+      <c r="U54" s="2"/>
+      <c r="V54" s="2"/>
+      <c r="W54" s="2"/>
+      <c r="X54" s="2"/>
+      <c r="Y54" s="2"/>
+      <c r="Z54" s="2"/>
+      <c r="AA54" s="2"/>
+      <c r="AB54" s="2"/>
+      <c r="AC54" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
         <v>2018</v>
       </c>
-      <c r="N55" s="1"/>
-    </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="2"/>
+      <c r="S55" s="2"/>
+      <c r="T55" s="2"/>
+      <c r="U55" s="2"/>
+      <c r="V55" s="2"/>
+      <c r="W55" s="2"/>
+      <c r="X55" s="2"/>
+      <c r="Y55" s="2"/>
+      <c r="Z55" s="2"/>
+      <c r="AA55" s="2"/>
+      <c r="AB55" s="2"/>
+      <c r="AC55" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
         <v>2019</v>
       </c>
-      <c r="N56" s="1"/>
-    </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="2"/>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
+      <c r="U56" s="2"/>
+      <c r="V56" s="2"/>
+      <c r="W56" s="2"/>
+      <c r="X56" s="2"/>
+      <c r="Y56" s="2"/>
+      <c r="Z56" s="2"/>
+      <c r="AA56" s="2"/>
+      <c r="AB56" s="2"/>
+      <c r="AC56" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
         <v>2020</v>
       </c>
-      <c r="N57" s="1"/>
-      <c r="Z57">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2"/>
+      <c r="S57" s="2"/>
+      <c r="T57" s="2"/>
+      <c r="U57" s="2"/>
+      <c r="V57" s="2"/>
+      <c r="W57" s="2"/>
+      <c r="X57" s="2"/>
+      <c r="Y57" s="2"/>
+      <c r="Z57" s="2"/>
+      <c r="AA57" s="2"/>
+      <c r="AB57" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="AC57" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
         <v>2021</v>
       </c>
-      <c r="N58" s="1"/>
-    </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="7"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
+      <c r="R58" s="2"/>
+      <c r="S58" s="2"/>
+      <c r="T58" s="2"/>
+      <c r="U58" s="2"/>
+      <c r="V58" s="2"/>
+      <c r="W58" s="2"/>
+      <c r="X58" s="2"/>
+      <c r="Y58" s="2"/>
+      <c r="Z58" s="2"/>
+      <c r="AA58" s="2"/>
+      <c r="AB58" s="2"/>
+      <c r="AC58" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
         <v>2022</v>
       </c>
-      <c r="N59" s="1"/>
-    </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="2"/>
+      <c r="Q59" s="2"/>
+      <c r="R59" s="2"/>
+      <c r="S59" s="2"/>
+      <c r="T59" s="2"/>
+      <c r="U59" s="2"/>
+      <c r="V59" s="2"/>
+      <c r="W59" s="2"/>
+      <c r="X59" s="2"/>
+      <c r="Y59" s="2"/>
+      <c r="Z59" s="2"/>
+      <c r="AA59" s="2"/>
+      <c r="AB59" s="2"/>
+      <c r="AC59" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N60" s="1"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N61" s="1"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N62" s="1"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N63" s="1"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
       <c r="N64" s="1"/>
     </row>
     <row r="65" spans="14:14" x14ac:dyDescent="0.25">
@@ -2046,7 +3922,7 @@
     <hyperlink ref="K3" r:id="rId2" display="https://www.nfl.com/teams/indianapolis-colts/"/>
     <hyperlink ref="O3" r:id="rId3" display="https://www.nfl.com/teams/los-angeles-rams/"/>
     <hyperlink ref="J3" r:id="rId4" display="https://www.nfl.com/teams/green-bay-packers/"/>
-    <hyperlink ref="Y3" r:id="rId5" display="https://www.nfl.com/teams/tennessee-titans/"/>
+    <hyperlink ref="AA3" r:id="rId5" display="https://www.nfl.com/teams/tennessee-titans/"/>
     <hyperlink ref="F3" r:id="rId6" display="https://www.nfl.com/teams/cleveland-browns/"/>
     <hyperlink ref="G3" r:id="rId7" display="https://www.nfl.com/teams/dallas-cowboys/"/>
     <hyperlink ref="L3" r:id="rId8" display="https://www.nfl.com/teams/kansas-city-chiefs/"/>
@@ -2054,10 +3930,10 @@
     <hyperlink ref="U3" r:id="rId10" display="https://www.nfl.com/teams/new-york-jets/"/>
     <hyperlink ref="E3" r:id="rId11" display="https://www.nfl.com/teams/chicago-bears/"/>
     <hyperlink ref="T3" r:id="rId12" display="https://www.nfl.com/teams/new-york-giants/"/>
-    <hyperlink ref="X3" r:id="rId13" display="https://www.nfl.com/teams/san-francisco-49ers/"/>
+    <hyperlink ref="Y3" r:id="rId13" display="https://www.nfl.com/teams/san-francisco-49ers/"/>
     <hyperlink ref="B3" r:id="rId14" display="https://www.nfl.com/teams/arizona-cardinals/"/>
     <hyperlink ref="V3" r:id="rId15" display="https://www.nfl.com/teams/philadelphia-eagles/"/>
-    <hyperlink ref="Z3" r:id="rId16" display="https://www.nfl.com/teams/washington-commanders/"/>
+    <hyperlink ref="AB3" r:id="rId16" display="https://www.nfl.com/teams/washington-commanders/"/>
     <hyperlink ref="I3" r:id="rId17" display="https://www.nfl.com/teams/detroit-lions/"/>
     <hyperlink ref="W3" r:id="rId18" display="https://www.nfl.com/teams/pittsburgh-steelers/"/>
     <hyperlink ref="D3" r:id="rId19" display="https://www.nfl.com/teams/buffalo-bills/"/>

</xml_diff>

<commit_message>
Populated playoff data through 1991
</commit_message>
<xml_diff>
--- a/NFL_playoff_wins.xlsx
+++ b/NFL_playoff_wins.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Year</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Wildcard implemented</t>
-  </si>
-  <si>
     <t>Number of playoff wins per team per year</t>
   </si>
   <si>
@@ -121,12 +118,27 @@
   <si>
     <t>San Diego Chargers</t>
   </si>
+  <si>
+    <t>Cincinnati Bengals</t>
+  </si>
+  <si>
+    <t>Seattle Seahawks</t>
+  </si>
+  <si>
+    <t>2 Wildcard games</t>
+  </si>
+  <si>
+    <t>4 Wildcard games</t>
+  </si>
+  <si>
+    <t>8 Wildcard games</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +165,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,7 +220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -220,6 +240,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -243,13 +267,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -287,13 +311,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -331,13 +355,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -375,13 +399,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -419,13 +443,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -463,13 +487,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -507,13 +531,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -551,13 +575,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -595,13 +619,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -639,13 +663,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -683,13 +707,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -727,13 +751,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -771,13 +795,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -815,13 +839,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -859,13 +883,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -903,13 +927,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -947,13 +971,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -991,13 +1015,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>70</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1035,13 +1059,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>70</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1079,13 +1103,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1123,13 +1147,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1167,13 +1191,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1211,13 +1235,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1255,13 +1279,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1299,13 +1323,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>77</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1607,30 +1631,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD77"/>
+  <dimension ref="A1:AF77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="21" width="10.140625" customWidth="1"/>
-    <col min="22" max="22" width="15.5703125" customWidth="1"/>
-    <col min="23" max="24" width="10.140625" customWidth="1"/>
-    <col min="25" max="26" width="15.85546875" customWidth="1"/>
-    <col min="27" max="27" width="10.140625" customWidth="1"/>
-    <col min="28" max="28" width="14.85546875" customWidth="1"/>
-    <col min="30" max="30" width="21.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.140625" style="8"/>
+    <col min="2" max="22" width="10.140625" customWidth="1"/>
+    <col min="23" max="23" width="15.5703125" customWidth="1"/>
+    <col min="24" max="25" width="10.140625" customWidth="1"/>
+    <col min="26" max="28" width="15.85546875" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" customWidth="1"/>
+    <col min="30" max="30" width="14.85546875" customWidth="1"/>
+    <col min="32" max="32" width="21.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="10.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" ht="45" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1647,82 +1671,88 @@
         <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="N3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="X3" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="Y3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Z3" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="AA3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AE3" t="s">
         <v>26</v>
       </c>
-      <c r="AD3" s="8" t="s">
+      <c r="AF3" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1967</v>
       </c>
@@ -1731,19 +1761,19 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="4">
+      <c r="J4" s="4"/>
+      <c r="K4" s="4">
         <v>3</v>
       </c>
-      <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="5"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
@@ -1757,12 +1787,14 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
-      <c r="AC4" s="9">
-        <f>SUM(B4:AB4)</f>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="9">
+        <f>SUM(B4:AD4)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1968</v>
       </c>
@@ -1770,17 +1802,17 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="4">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="4">
+      <c r="K5" s="4"/>
+      <c r="L5" s="4">
         <v>2</v>
       </c>
-      <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -1789,22 +1821,24 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
-      <c r="U5" s="4">
-        <v>1</v>
-      </c>
-      <c r="V5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4">
+        <v>1</v>
+      </c>
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
-      <c r="AC5" s="9">
-        <f t="shared" ref="AC5:AC59" si="0">SUM(B5:AB5)</f>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="9">
+        <f t="shared" ref="AE5:AE59" si="0">SUM(B5:AD5)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1969</v>
       </c>
@@ -1812,25 +1846,25 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="4">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="4">
-        <v>1</v>
-      </c>
-      <c r="M6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="4">
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4">
         <v>2</v>
       </c>
-      <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
@@ -1841,12 +1875,14 @@
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
-      <c r="AC6" s="9">
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1970</v>
       </c>
@@ -1855,20 +1891,20 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="4">
+      <c r="G7" s="4"/>
+      <c r="H7" s="4">
         <v>2</v>
       </c>
-      <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="4">
+      <c r="K7" s="4"/>
+      <c r="L7" s="4">
         <v>3</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4">
-        <v>1</v>
-      </c>
-      <c r="N7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4">
+        <v>1</v>
+      </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
@@ -1879,18 +1915,20 @@
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
-      <c r="Y7" s="4">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4">
+        <v>1</v>
+      </c>
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
-      <c r="AC7" s="9">
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1971</v>
       </c>
@@ -1899,23 +1937,23 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="4">
+      <c r="G8" s="4"/>
+      <c r="H8" s="4">
         <v>3</v>
       </c>
-      <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="4">
-        <v>1</v>
-      </c>
-      <c r="L8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4">
+        <v>1</v>
+      </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
-      <c r="P8" s="4">
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4">
         <v>2</v>
       </c>
-      <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
@@ -1923,18 +1961,20 @@
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
-      <c r="Y8" s="4">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4">
+        <v>1</v>
+      </c>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
-      <c r="AC8" s="9">
+      <c r="AC8" s="4"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1972</v>
       </c>
@@ -1943,10 +1983,10 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -1954,31 +1994,33 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="4">
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4">
         <v>3</v>
       </c>
-      <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
-      <c r="W9" s="4">
-        <v>1</v>
-      </c>
-      <c r="X9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4">
+        <v>1</v>
+      </c>
       <c r="Y9" s="4"/>
       <c r="Z9" s="4"/>
       <c r="AA9" s="4"/>
-      <c r="AB9" s="4">
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4">
         <v>2</v>
       </c>
-      <c r="AC9" s="9">
+      <c r="AE9" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1973</v>
       </c>
@@ -1987,26 +2029,26 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="4">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="4">
-        <v>1</v>
-      </c>
-      <c r="N10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4">
+        <v>1</v>
+      </c>
       <c r="O10" s="4"/>
-      <c r="P10" s="4">
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4">
         <v>3</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="R10" s="4">
         <v>2</v>
       </c>
-      <c r="R10" s="4"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
@@ -2017,12 +2059,14 @@
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
-      <c r="AC10" s="9">
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1974</v>
       </c>
@@ -2037,36 +2081,38 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="4">
-        <v>1</v>
-      </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4">
-        <v>1</v>
-      </c>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4">
+      <c r="M11" s="4"/>
+      <c r="N11" s="4">
+        <v>1</v>
+      </c>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4">
         <v>2</v>
       </c>
-      <c r="R11" s="4"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
-      <c r="W11" s="4">
+      <c r="W11" s="4"/>
+      <c r="X11" s="4">
         <v>3</v>
       </c>
-      <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
-      <c r="AC11" s="9">
+      <c r="AC11" s="4"/>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>1975</v>
       </c>
@@ -2075,42 +2121,44 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="4">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4">
         <v>2</v>
       </c>
-      <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="4">
-        <v>1</v>
-      </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4">
-        <v>1</v>
-      </c>
-      <c r="P12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4">
+        <v>1</v>
+      </c>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4">
+        <v>1</v>
+      </c>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
-      <c r="W12" s="4">
+      <c r="W12" s="4"/>
+      <c r="X12" s="4">
         <v>3</v>
       </c>
-      <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
       <c r="AA12" s="4"/>
       <c r="AB12" s="4"/>
-      <c r="AC12" s="9">
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>1976</v>
       </c>
@@ -2125,36 +2173,38 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="4">
+      <c r="M13" s="4"/>
+      <c r="N13" s="4">
         <v>3</v>
       </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4">
-        <v>1</v>
-      </c>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4">
+      <c r="O13" s="4"/>
+      <c r="P13" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4">
         <v>2</v>
       </c>
-      <c r="R13" s="4"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
-      <c r="W13" s="4">
-        <v>1</v>
-      </c>
-      <c r="X13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4">
+        <v>1</v>
+      </c>
       <c r="Y13" s="4"/>
       <c r="Z13" s="4"/>
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
-      <c r="AC13" s="9">
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>1977</v>
       </c>
@@ -2163,26 +2213,26 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4">
         <v>3</v>
       </c>
-      <c r="H14" s="4">
+      <c r="I14" s="4">
         <v>2</v>
       </c>
-      <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="4">
-        <v>1</v>
-      </c>
-      <c r="N14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4">
+        <v>1</v>
+      </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="4">
-        <v>1</v>
-      </c>
-      <c r="R14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4">
+        <v>1</v>
+      </c>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
@@ -2193,12 +2243,14 @@
       <c r="Z14" s="4"/>
       <c r="AA14" s="4"/>
       <c r="AB14" s="4"/>
-      <c r="AC14" s="9">
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>1978</v>
       </c>
@@ -2209,45 +2261,47 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4">
+      <c r="G15" s="4"/>
+      <c r="H15" s="4">
         <v>2</v>
       </c>
-      <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="4">
-        <v>1</v>
-      </c>
-      <c r="P15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4">
+        <v>1</v>
+      </c>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
-      <c r="W15" s="4">
+      <c r="W15" s="4"/>
+      <c r="X15" s="4">
         <v>3</v>
       </c>
-      <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
       <c r="Z15" s="4"/>
-      <c r="AA15" s="4">
+      <c r="AA15" s="4"/>
+      <c r="AB15" s="4"/>
+      <c r="AC15" s="4">
         <v>2</v>
       </c>
-      <c r="AB15" s="4"/>
-      <c r="AC15" s="9">
+      <c r="AD15" s="4"/>
+      <c r="AE15" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AD15" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF15" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>1979</v>
       </c>
@@ -2264,36 +2318,41 @@
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
-      <c r="O16" s="4">
+      <c r="O16" s="4"/>
+      <c r="P16" s="4">
         <v>2</v>
       </c>
-      <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
-      <c r="V16" s="4">
-        <v>1</v>
-      </c>
+      <c r="V16" s="4"/>
       <c r="W16" s="4">
+        <v>1</v>
+      </c>
+      <c r="X16" s="4">
         <v>3</v>
       </c>
-      <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
-      <c r="Z16" s="4">
-        <v>1</v>
-      </c>
-      <c r="AA16" s="4">
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC16" s="4">
         <v>2</v>
       </c>
-      <c r="AB16" s="4"/>
-      <c r="AC16" s="9">
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AF16" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>1980</v>
       </c>
@@ -2302,18 +2361,18 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="4">
+      <c r="G17" s="4"/>
+      <c r="H17" s="4">
         <v>2</v>
       </c>
-      <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="4">
+      <c r="M17" s="4"/>
+      <c r="N17" s="4">
         <v>4</v>
       </c>
-      <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
@@ -2321,419 +2380,610 @@
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
-      <c r="V17" s="4">
+      <c r="V17" s="4"/>
+      <c r="W17" s="4">
         <v>2</v>
       </c>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4">
+        <v>1</v>
+      </c>
       <c r="Z17" s="4"/>
       <c r="AA17" s="4"/>
       <c r="AB17" s="4"/>
-      <c r="AC17" s="9">
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="AF17" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>1981</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-      <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
-      <c r="Z18" s="2"/>
-      <c r="AA18" s="2"/>
-      <c r="AB18" s="2"/>
-      <c r="AC18" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4">
+        <v>2</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4">
+        <v>1</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4">
+        <v>1</v>
+      </c>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4">
+        <v>1</v>
+      </c>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4">
+        <v>3</v>
+      </c>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AF18" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>1982</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-      <c r="X19" s="2"/>
-      <c r="Y19" s="2"/>
-      <c r="Z19" s="2"/>
-      <c r="AA19" s="2"/>
-      <c r="AB19" s="2"/>
-      <c r="AC19" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4">
+        <v>2</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4">
+        <v>1</v>
+      </c>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4">
+        <v>1</v>
+      </c>
+      <c r="O19" s="4">
+        <v>1</v>
+      </c>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4">
+        <v>3</v>
+      </c>
+      <c r="R19" s="4">
+        <v>1</v>
+      </c>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4">
+        <v>2</v>
+      </c>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4">
+        <v>4</v>
+      </c>
+      <c r="AE19" s="9">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="AF19" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
         <v>1983</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="X20" s="2"/>
-      <c r="Y20" s="2"/>
-      <c r="Z20" s="2"/>
-      <c r="AA20" s="2"/>
-      <c r="AB20" s="2"/>
-      <c r="AC20" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4">
+        <v>3</v>
+      </c>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="4"/>
+      <c r="AD20" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE20" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AF20" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>1984</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-      <c r="X21" s="2"/>
-      <c r="Y21" s="2"/>
-      <c r="Z21" s="2"/>
-      <c r="AA21" s="2"/>
-      <c r="AB21" s="2"/>
-      <c r="AC21" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4">
+        <v>2</v>
+      </c>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4">
+        <v>1</v>
+      </c>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4">
+        <v>3</v>
+      </c>
+      <c r="AA21" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
+      <c r="AE21" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AF21" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>1985</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
-      <c r="X22" s="2"/>
-      <c r="Y22" s="2"/>
-      <c r="Z22" s="2"/>
-      <c r="AA22" s="2"/>
-      <c r="AB22" s="2"/>
-      <c r="AC22" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4">
+        <v>3</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>1</v>
+      </c>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4">
+        <v>3</v>
+      </c>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4">
+        <v>1</v>
+      </c>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="4"/>
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AF22" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>1986</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
-      <c r="X23" s="2"/>
-      <c r="Y23" s="2"/>
-      <c r="Z23" s="2"/>
-      <c r="AA23" s="2"/>
-      <c r="AB23" s="2"/>
-      <c r="AC23" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4">
+        <v>1</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4">
+        <v>2</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4">
+        <v>3</v>
+      </c>
+      <c r="V23" s="4">
+        <v>1</v>
+      </c>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="4"/>
+      <c r="AA23" s="4"/>
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="4"/>
+      <c r="AD23" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE23" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AF23" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>1987</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
-      <c r="X24" s="2"/>
-      <c r="Y24" s="2"/>
-      <c r="Z24" s="2"/>
-      <c r="AA24" s="2"/>
-      <c r="AB24" s="2"/>
-      <c r="AC24" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4">
+        <v>1</v>
+      </c>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4">
+        <v>2</v>
+      </c>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4">
+        <v>2</v>
+      </c>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="4"/>
+      <c r="W24" s="4"/>
+      <c r="X24" s="4"/>
+      <c r="Y24" s="4"/>
+      <c r="Z24" s="4"/>
+      <c r="AA24" s="4"/>
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD24" s="4">
+        <v>3</v>
+      </c>
+      <c r="AE24" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AF24" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>1988</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
-      <c r="X25" s="2"/>
-      <c r="Y25" s="2"/>
-      <c r="Z25" s="2"/>
-      <c r="AA25" s="2"/>
-      <c r="AB25" s="2"/>
-      <c r="AC25" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
+      <c r="F25" s="4">
+        <v>2</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4">
+        <v>1</v>
+      </c>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="4">
+        <v>3</v>
+      </c>
+      <c r="AA25" s="4"/>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD25" s="4"/>
+      <c r="AE25" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AF25" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
         <v>1989</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-      <c r="U26" s="2"/>
-      <c r="V26" s="2"/>
-      <c r="W26" s="2"/>
-      <c r="X26" s="2"/>
-      <c r="Y26" s="2"/>
-      <c r="Z26" s="2"/>
-      <c r="AA26" s="2"/>
-      <c r="AB26" s="2"/>
-      <c r="AC26" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4">
+        <v>1</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4">
+        <v>2</v>
+      </c>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4">
+        <v>3</v>
+      </c>
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="4"/>
+      <c r="AD26" s="4"/>
+      <c r="AE26" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="AF26" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
         <v>1990</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
-      <c r="W27" s="2"/>
-      <c r="X27" s="2"/>
-      <c r="Y27" s="2"/>
-      <c r="Z27" s="2"/>
-      <c r="AA27" s="2"/>
-      <c r="AB27" s="2"/>
-      <c r="AC27" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4">
+        <v>2</v>
+      </c>
+      <c r="E27" s="4">
+        <v>1</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4">
+        <v>1</v>
+      </c>
+      <c r="O27" s="11"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4">
+        <v>1</v>
+      </c>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4">
+        <v>3</v>
+      </c>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="4"/>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="4"/>
+      <c r="AD27" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE27" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AF27" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
         <v>1991</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-      <c r="U28" s="2"/>
-      <c r="V28" s="2"/>
-      <c r="W28" s="2"/>
-      <c r="X28" s="2"/>
-      <c r="Y28" s="2"/>
-      <c r="Z28" s="2"/>
-      <c r="AA28" s="2"/>
-      <c r="AB28" s="2"/>
-      <c r="AC28" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
+      <c r="D28" s="4">
+        <v>2</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4">
+        <v>1</v>
+      </c>
+      <c r="I28" s="4">
+        <v>1</v>
+      </c>
+      <c r="J28" s="4">
+        <v>1</v>
+      </c>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4">
+        <v>1</v>
+      </c>
+      <c r="N28" s="4"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="4"/>
+      <c r="AB28" s="4"/>
+      <c r="AC28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD28" s="4">
+        <v>3</v>
+      </c>
+      <c r="AE28" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>1992</v>
       </c>
@@ -2749,8 +2999,8 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="6"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
@@ -2764,12 +3014,14 @@
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
-      <c r="AC29" s="9">
+      <c r="AC29" s="2"/>
+      <c r="AD29" s="2"/>
+      <c r="AE29" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>1993</v>
       </c>
@@ -2785,8 +3037,8 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="6"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
@@ -2800,12 +3052,14 @@
       <c r="Z30" s="2"/>
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
-      <c r="AC30" s="9">
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>1994</v>
       </c>
@@ -2821,8 +3075,8 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="6"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
@@ -2836,12 +3090,14 @@
       <c r="Z31" s="2"/>
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
-      <c r="AC31" s="9">
+      <c r="AC31" s="2"/>
+      <c r="AD31" s="2"/>
+      <c r="AE31" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>1995</v>
       </c>
@@ -2857,8 +3113,8 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="6"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
@@ -2872,12 +3128,14 @@
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
-      <c r="AC32" s="9">
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="2"/>
+      <c r="AE32" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>1996</v>
       </c>
@@ -2893,8 +3151,8 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="6"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
@@ -2908,12 +3166,14 @@
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
-      <c r="AC33" s="9">
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="2"/>
+      <c r="AE33" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>1997</v>
       </c>
@@ -2929,8 +3189,8 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="6"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
@@ -2944,12 +3204,14 @@
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
-      <c r="AC34" s="9">
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="2"/>
+      <c r="AE34" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>1998</v>
       </c>
@@ -2965,8 +3227,8 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="6"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
@@ -2980,12 +3242,14 @@
       <c r="Z35" s="2"/>
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
-      <c r="AC35" s="9">
+      <c r="AC35" s="2"/>
+      <c r="AD35" s="2"/>
+      <c r="AE35" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>1999</v>
       </c>
@@ -3001,8 +3265,8 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="6"/>
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
@@ -3016,12 +3280,14 @@
       <c r="Z36" s="2"/>
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
-      <c r="AC36" s="9">
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="2"/>
+      <c r="AE36" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>2000</v>
       </c>
@@ -3037,8 +3303,8 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="6"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
@@ -3052,12 +3318,14 @@
       <c r="Z37" s="2"/>
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
-      <c r="AC37" s="9">
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="2"/>
+      <c r="AE37" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>2001</v>
       </c>
@@ -3073,8 +3341,8 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="6"/>
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
@@ -3088,12 +3356,14 @@
       <c r="Z38" s="2"/>
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
-      <c r="AC38" s="9">
+      <c r="AC38" s="2"/>
+      <c r="AD38" s="2"/>
+      <c r="AE38" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>2002</v>
       </c>
@@ -3109,8 +3379,8 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="6"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
@@ -3124,12 +3394,14 @@
       <c r="Z39" s="2"/>
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
-      <c r="AC39" s="9">
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="2"/>
+      <c r="AE39" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>2003</v>
       </c>
@@ -3145,8 +3417,8 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="6"/>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
@@ -3160,12 +3432,14 @@
       <c r="Z40" s="2"/>
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
-      <c r="AC40" s="9">
+      <c r="AC40" s="2"/>
+      <c r="AD40" s="2"/>
+      <c r="AE40" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>2004</v>
       </c>
@@ -3181,8 +3455,8 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="6"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
@@ -3196,12 +3470,14 @@
       <c r="Z41" s="2"/>
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
-      <c r="AC41" s="9">
+      <c r="AC41" s="2"/>
+      <c r="AD41" s="2"/>
+      <c r="AE41" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>2005</v>
       </c>
@@ -3217,8 +3493,8 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="6"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
@@ -3231,15 +3507,17 @@
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
       <c r="AA42" s="2"/>
-      <c r="AB42" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC42" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB42" s="2"/>
+      <c r="AC42" s="2"/>
+      <c r="AD42" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE42" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>2006</v>
       </c>
@@ -3255,8 +3533,8 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="6"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
@@ -3270,12 +3548,14 @@
       <c r="Z43" s="2"/>
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
-      <c r="AC43" s="9">
+      <c r="AC43" s="2"/>
+      <c r="AD43" s="2"/>
+      <c r="AE43" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>2007</v>
       </c>
@@ -3291,8 +3571,8 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
-      <c r="N44" s="6"/>
-      <c r="O44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="6"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
@@ -3305,15 +3585,17 @@
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
       <c r="AA44" s="2"/>
-      <c r="AB44" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC44" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB44" s="2"/>
+      <c r="AC44" s="2"/>
+      <c r="AD44" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE44" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>2008</v>
       </c>
@@ -3329,8 +3611,8 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="6"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
@@ -3344,12 +3626,14 @@
       <c r="Z45" s="2"/>
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
-      <c r="AC45" s="9">
+      <c r="AC45" s="2"/>
+      <c r="AD45" s="2"/>
+      <c r="AE45" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>2009</v>
       </c>
@@ -3365,8 +3649,8 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
-      <c r="N46" s="6"/>
-      <c r="O46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="6"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
@@ -3380,12 +3664,14 @@
       <c r="Z46" s="2"/>
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
-      <c r="AC46" s="9">
+      <c r="AC46" s="2"/>
+      <c r="AD46" s="2"/>
+      <c r="AE46" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>2010</v>
       </c>
@@ -3401,8 +3687,8 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
-      <c r="N47" s="6"/>
-      <c r="O47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="6"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
@@ -3416,12 +3702,14 @@
       <c r="Z47" s="2"/>
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
-      <c r="AC47" s="9">
+      <c r="AC47" s="2"/>
+      <c r="AD47" s="2"/>
+      <c r="AE47" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>2011</v>
       </c>
@@ -3437,8 +3725,8 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
-      <c r="N48" s="6"/>
-      <c r="O48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="6"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
@@ -3452,12 +3740,14 @@
       <c r="Z48" s="2"/>
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
-      <c r="AC48" s="9">
+      <c r="AC48" s="2"/>
+      <c r="AD48" s="2"/>
+      <c r="AE48" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>2012</v>
       </c>
@@ -3473,8 +3763,8 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
-      <c r="N49" s="6"/>
-      <c r="O49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="6"/>
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
@@ -3487,15 +3777,17 @@
       <c r="Y49" s="2"/>
       <c r="Z49" s="2"/>
       <c r="AA49" s="2"/>
-      <c r="AB49" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC49" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB49" s="2"/>
+      <c r="AC49" s="2"/>
+      <c r="AD49" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE49" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>2013</v>
       </c>
@@ -3511,8 +3803,8 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
-      <c r="N50" s="6"/>
-      <c r="O50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="6"/>
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
@@ -3526,12 +3818,14 @@
       <c r="Z50" s="2"/>
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
-      <c r="AC50" s="9">
+      <c r="AC50" s="2"/>
+      <c r="AD50" s="2"/>
+      <c r="AE50" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>2014</v>
       </c>
@@ -3547,8 +3841,8 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="6"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
@@ -3562,12 +3856,14 @@
       <c r="Z51" s="2"/>
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
-      <c r="AC51" s="9">
+      <c r="AC51" s="2"/>
+      <c r="AD51" s="2"/>
+      <c r="AE51" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>2015</v>
       </c>
@@ -3597,15 +3893,17 @@
       <c r="Y52" s="2"/>
       <c r="Z52" s="2"/>
       <c r="AA52" s="2"/>
-      <c r="AB52" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC52" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB52" s="2"/>
+      <c r="AC52" s="2"/>
+      <c r="AD52" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE52" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>2016</v>
       </c>
@@ -3621,8 +3919,8 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
-      <c r="N53" s="7"/>
-      <c r="O53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="7"/>
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
@@ -3636,12 +3934,14 @@
       <c r="Z53" s="2"/>
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
-      <c r="AC53" s="9">
+      <c r="AC53" s="2"/>
+      <c r="AD53" s="2"/>
+      <c r="AE53" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>2017</v>
       </c>
@@ -3657,8 +3957,8 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
-      <c r="N54" s="7"/>
-      <c r="O54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="7"/>
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
@@ -3672,12 +3972,14 @@
       <c r="Z54" s="2"/>
       <c r="AA54" s="2"/>
       <c r="AB54" s="2"/>
-      <c r="AC54" s="9">
+      <c r="AC54" s="2"/>
+      <c r="AD54" s="2"/>
+      <c r="AE54" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>2018</v>
       </c>
@@ -3693,8 +3995,8 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
-      <c r="N55" s="7"/>
-      <c r="O55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="7"/>
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
@@ -3708,12 +4010,14 @@
       <c r="Z55" s="2"/>
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
-      <c r="AC55" s="9">
+      <c r="AC55" s="2"/>
+      <c r="AD55" s="2"/>
+      <c r="AE55" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>2019</v>
       </c>
@@ -3729,8 +4033,8 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
-      <c r="N56" s="7"/>
-      <c r="O56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="7"/>
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
@@ -3744,12 +4048,14 @@
       <c r="Z56" s="2"/>
       <c r="AA56" s="2"/>
       <c r="AB56" s="2"/>
-      <c r="AC56" s="9">
+      <c r="AC56" s="2"/>
+      <c r="AD56" s="2"/>
+      <c r="AE56" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>2020</v>
       </c>
@@ -3765,8 +4071,8 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
-      <c r="N57" s="7"/>
-      <c r="O57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="7"/>
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
@@ -3779,15 +4085,17 @@
       <c r="Y57" s="2"/>
       <c r="Z57" s="2"/>
       <c r="AA57" s="2"/>
-      <c r="AB57" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC57" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB57" s="2"/>
+      <c r="AC57" s="2"/>
+      <c r="AD57" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE57" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>2021</v>
       </c>
@@ -3803,8 +4111,8 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
-      <c r="N58" s="7"/>
-      <c r="O58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="7"/>
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
@@ -3818,12 +4126,14 @@
       <c r="Z58" s="2"/>
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
-      <c r="AC58" s="9">
+      <c r="AC58" s="2"/>
+      <c r="AD58" s="2"/>
+      <c r="AE58" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>2022</v>
       </c>
@@ -3839,8 +4149,8 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
-      <c r="N59" s="7"/>
-      <c r="O59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="7"/>
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
@@ -3854,94 +4164,96 @@
       <c r="Z59" s="2"/>
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
-      <c r="AC59" s="9">
+      <c r="AC59" s="2"/>
+      <c r="AD59" s="2"/>
+      <c r="AE59" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="N60" s="1"/>
-    </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="N61" s="1"/>
-    </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="N62" s="1"/>
-    </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="N63" s="1"/>
-    </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="N64" s="1"/>
-    </row>
-    <row r="65" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N65" s="1"/>
-    </row>
-    <row r="66" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N66" s="1"/>
-    </row>
-    <row r="67" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N67" s="1"/>
-    </row>
-    <row r="68" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N68" s="1"/>
-    </row>
-    <row r="69" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N69" s="1"/>
-    </row>
-    <row r="70" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N70" s="1"/>
-    </row>
-    <row r="71" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N71" s="1"/>
-    </row>
-    <row r="72" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N72" s="1"/>
-    </row>
-    <row r="73" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N73" s="1"/>
-    </row>
-    <row r="74" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N74" s="1"/>
-    </row>
-    <row r="75" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N75" s="1"/>
-    </row>
-    <row r="76" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N76" s="1"/>
-    </row>
-    <row r="77" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N77" s="1"/>
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="O60" s="1"/>
+    </row>
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="O61" s="1"/>
+    </row>
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="O62" s="1"/>
+    </row>
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="O63" s="1"/>
+    </row>
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="O64" s="1"/>
+    </row>
+    <row r="65" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O65" s="1"/>
+    </row>
+    <row r="66" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O66" s="1"/>
+    </row>
+    <row r="67" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O67" s="1"/>
+    </row>
+    <row r="68" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O68" s="1"/>
+    </row>
+    <row r="69" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O69" s="1"/>
+    </row>
+    <row r="70" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O70" s="1"/>
+    </row>
+    <row r="71" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O71" s="1"/>
+    </row>
+    <row r="72" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O72" s="1"/>
+    </row>
+    <row r="73" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O73" s="1"/>
+    </row>
+    <row r="74" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O74" s="1"/>
+    </row>
+    <row r="75" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O75" s="1"/>
+    </row>
+    <row r="76" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O76" s="1"/>
+    </row>
+    <row r="77" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O77" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="N1:N76">
-    <sortCondition ref="N1"/>
+  <sortState ref="O1:O76">
+    <sortCondition ref="O1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1" display="https://www.nfl.com/teams/las-vegas-raiders/"/>
-    <hyperlink ref="K3" r:id="rId2" display="https://www.nfl.com/teams/indianapolis-colts/"/>
-    <hyperlink ref="O3" r:id="rId3" display="https://www.nfl.com/teams/los-angeles-rams/"/>
-    <hyperlink ref="J3" r:id="rId4" display="https://www.nfl.com/teams/green-bay-packers/"/>
-    <hyperlink ref="AA3" r:id="rId5" display="https://www.nfl.com/teams/tennessee-titans/"/>
-    <hyperlink ref="F3" r:id="rId6" display="https://www.nfl.com/teams/cleveland-browns/"/>
-    <hyperlink ref="G3" r:id="rId7" display="https://www.nfl.com/teams/dallas-cowboys/"/>
-    <hyperlink ref="L3" r:id="rId8" display="https://www.nfl.com/teams/kansas-city-chiefs/"/>
-    <hyperlink ref="N3" r:id="rId9" display="https://www.nfl.com/teams/los-angeles-chargers/"/>
-    <hyperlink ref="U3" r:id="rId10" display="https://www.nfl.com/teams/new-york-jets/"/>
+    <hyperlink ref="N3" r:id="rId1" display="https://www.nfl.com/teams/las-vegas-raiders/"/>
+    <hyperlink ref="L3" r:id="rId2" display="https://www.nfl.com/teams/indianapolis-colts/"/>
+    <hyperlink ref="P3" r:id="rId3" display="https://www.nfl.com/teams/los-angeles-rams/"/>
+    <hyperlink ref="K3" r:id="rId4" display="https://www.nfl.com/teams/green-bay-packers/"/>
+    <hyperlink ref="AC3" r:id="rId5" display="https://www.nfl.com/teams/tennessee-titans/"/>
+    <hyperlink ref="G3" r:id="rId6" display="https://www.nfl.com/teams/cleveland-browns/"/>
+    <hyperlink ref="H3" r:id="rId7" display="https://www.nfl.com/teams/dallas-cowboys/"/>
+    <hyperlink ref="M3" r:id="rId8" display="https://www.nfl.com/teams/kansas-city-chiefs/"/>
+    <hyperlink ref="O3" r:id="rId9" display="https://www.nfl.com/teams/los-angeles-chargers/"/>
+    <hyperlink ref="V3" r:id="rId10" display="https://www.nfl.com/teams/new-york-jets/"/>
     <hyperlink ref="E3" r:id="rId11" display="https://www.nfl.com/teams/chicago-bears/"/>
-    <hyperlink ref="T3" r:id="rId12" display="https://www.nfl.com/teams/new-york-giants/"/>
-    <hyperlink ref="Y3" r:id="rId13" display="https://www.nfl.com/teams/san-francisco-49ers/"/>
+    <hyperlink ref="U3" r:id="rId12" display="https://www.nfl.com/teams/new-york-giants/"/>
+    <hyperlink ref="Z3" r:id="rId13" display="https://www.nfl.com/teams/san-francisco-49ers/"/>
     <hyperlink ref="B3" r:id="rId14" display="https://www.nfl.com/teams/arizona-cardinals/"/>
-    <hyperlink ref="V3" r:id="rId15" display="https://www.nfl.com/teams/philadelphia-eagles/"/>
-    <hyperlink ref="AB3" r:id="rId16" display="https://www.nfl.com/teams/washington-commanders/"/>
-    <hyperlink ref="I3" r:id="rId17" display="https://www.nfl.com/teams/detroit-lions/"/>
-    <hyperlink ref="W3" r:id="rId18" display="https://www.nfl.com/teams/pittsburgh-steelers/"/>
+    <hyperlink ref="W3" r:id="rId15" display="https://www.nfl.com/teams/philadelphia-eagles/"/>
+    <hyperlink ref="AD3" r:id="rId16" display="https://www.nfl.com/teams/washington-commanders/"/>
+    <hyperlink ref="J3" r:id="rId17" display="https://www.nfl.com/teams/detroit-lions/"/>
+    <hyperlink ref="X3" r:id="rId18" display="https://www.nfl.com/teams/pittsburgh-steelers/"/>
     <hyperlink ref="D3" r:id="rId19" display="https://www.nfl.com/teams/buffalo-bills/"/>
-    <hyperlink ref="P3" r:id="rId20" display="https://www.nfl.com/teams/miami-dolphins/"/>
-    <hyperlink ref="Q3" r:id="rId21" display="https://www.nfl.com/teams/minnesota-vikings/"/>
-    <hyperlink ref="R3" r:id="rId22" display="https://www.nfl.com/teams/new-england-patriots/"/>
-    <hyperlink ref="H3" r:id="rId23" display="https://www.nfl.com/teams/denver-broncos/"/>
-    <hyperlink ref="S3" r:id="rId24" display="https://www.nfl.com/teams/new-orleans-saints/"/>
+    <hyperlink ref="Q3" r:id="rId20" display="https://www.nfl.com/teams/miami-dolphins/"/>
+    <hyperlink ref="R3" r:id="rId21" display="https://www.nfl.com/teams/minnesota-vikings/"/>
+    <hyperlink ref="S3" r:id="rId22" display="https://www.nfl.com/teams/new-england-patriots/"/>
+    <hyperlink ref="I3" r:id="rId23" display="https://www.nfl.com/teams/denver-broncos/"/>
+    <hyperlink ref="T3" r:id="rId24" display="https://www.nfl.com/teams/new-orleans-saints/"/>
     <hyperlink ref="C3" r:id="rId25" display="https://www.nfl.com/teams/atlanta-falcons/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Populated playoff data through 2001
</commit_message>
<xml_diff>
--- a/NFL_playoff_wins.xlsx
+++ b/NFL_playoff_wins.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>Year</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>8 Wildcard games</t>
+  </si>
+  <si>
+    <t>Carolina Panthers</t>
+  </si>
+  <si>
+    <t>Jacksonville Jaguars</t>
+  </si>
+  <si>
+    <t>Baltimore Ravens</t>
   </si>
 </sst>
 </file>
@@ -267,13 +276,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -311,13 +320,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -355,13 +364,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -399,13 +408,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -443,13 +452,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -487,13 +496,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -531,13 +540,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -575,13 +584,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -619,13 +628,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -663,13 +672,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -707,13 +716,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -751,13 +760,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -795,13 +804,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -839,13 +848,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -883,13 +892,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -927,13 +936,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -971,13 +980,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1015,13 +1024,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>70</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1059,13 +1068,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>70</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1103,13 +1112,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1147,13 +1156,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1191,13 +1200,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1235,13 +1244,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1279,13 +1288,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1323,13 +1332,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>77</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1631,30 +1640,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF77"/>
+  <dimension ref="A1:AI77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="T45" sqref="T45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="22" width="10.140625" customWidth="1"/>
-    <col min="23" max="23" width="15.5703125" customWidth="1"/>
-    <col min="24" max="25" width="10.140625" customWidth="1"/>
-    <col min="26" max="28" width="15.85546875" customWidth="1"/>
-    <col min="29" max="29" width="10.140625" customWidth="1"/>
-    <col min="30" max="30" width="14.85546875" customWidth="1"/>
-    <col min="32" max="32" width="21.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="10.140625" style="8"/>
+    <col min="2" max="25" width="10.140625" customWidth="1"/>
+    <col min="26" max="26" width="15.5703125" customWidth="1"/>
+    <col min="27" max="28" width="10.140625" customWidth="1"/>
+    <col min="29" max="31" width="15.85546875" customWidth="1"/>
+    <col min="32" max="32" width="10.140625" customWidth="1"/>
+    <col min="33" max="33" width="14.85546875" customWidth="1"/>
+    <col min="35" max="35" width="21.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="10.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1665,94 +1674,103 @@
         <v>25</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="O3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AH3" t="s">
         <v>26</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AI3" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1967</v>
       </c>
@@ -1762,21 +1780,21 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="4">
-        <v>1</v>
-      </c>
+      <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4">
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4">
         <v>3</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="5"/>
+      <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
+      <c r="R4" s="5"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
@@ -1789,12 +1807,15 @@
       <c r="AB4" s="4"/>
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>
-      <c r="AE4" s="9">
-        <f>SUM(B4:AD4)</f>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="9">
+        <f>SUM(B4:AG4)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1968</v>
       </c>
@@ -1803,18 +1824,18 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
+      <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="4">
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4">
         <v>2</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
@@ -1822,23 +1843,26 @@
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
-      <c r="V5" s="4">
-        <v>1</v>
-      </c>
+      <c r="V5" s="4"/>
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
+      <c r="Y5" s="4">
+        <v>1</v>
+      </c>
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
-      <c r="AE5" s="9">
-        <f t="shared" ref="AE5:AE59" si="0">SUM(B5:AD5)</f>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="9">
+        <f t="shared" ref="AH5:AH59" si="0">SUM(B5:AG5)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1969</v>
       </c>
@@ -1847,27 +1871,27 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="4">
-        <v>1</v>
-      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="4">
-        <v>1</v>
-      </c>
+      <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
+      <c r="P6" s="4">
+        <v>1</v>
+      </c>
       <c r="Q6" s="4"/>
-      <c r="R6" s="4">
-        <v>2</v>
-      </c>
+      <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
+      <c r="U6" s="4">
+        <v>2</v>
+      </c>
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
@@ -1877,12 +1901,15 @@
       <c r="AB6" s="4"/>
       <c r="AC6" s="4"/>
       <c r="AD6" s="4"/>
-      <c r="AE6" s="9">
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1970</v>
       </c>
@@ -1892,22 +1919,22 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="4">
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4">
         <v>2</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="4">
-        <v>3</v>
-      </c>
+      <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
+      <c r="Q7" s="4">
+        <v>1</v>
+      </c>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
@@ -1916,19 +1943,22 @@
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
-      <c r="Z7" s="4">
-        <v>1</v>
-      </c>
+      <c r="Z7" s="4"/>
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
-      <c r="AC7" s="4"/>
+      <c r="AC7" s="4">
+        <v>1</v>
+      </c>
       <c r="AD7" s="4"/>
-      <c r="AE7" s="9">
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="4"/>
+      <c r="AH7" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1971</v>
       </c>
@@ -1938,43 +1968,46 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="4">
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4">
         <v>3</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="4">
-        <v>1</v>
-      </c>
+      <c r="L8" s="4"/>
       <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
+      <c r="N8" s="4">
+        <v>1</v>
+      </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="4">
-        <v>2</v>
-      </c>
+      <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
+      <c r="T8" s="4">
+        <v>2</v>
+      </c>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
-      <c r="Z8" s="4">
-        <v>1</v>
-      </c>
+      <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
-      <c r="AC8" s="4"/>
+      <c r="AC8" s="4">
+        <v>1</v>
+      </c>
       <c r="AD8" s="4"/>
-      <c r="AE8" s="9">
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="4"/>
+      <c r="AH8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1972</v>
       </c>
@@ -1984,43 +2017,46 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="4">
-        <v>1</v>
-      </c>
+      <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="J9" s="4">
+        <v>1</v>
+      </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-      <c r="Q9" s="4">
-        <v>3</v>
-      </c>
+      <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
+      <c r="T9" s="4">
+        <v>3</v>
+      </c>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
-      <c r="X9" s="4">
-        <v>1</v>
-      </c>
+      <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
       <c r="Z9" s="4"/>
-      <c r="AA9" s="4"/>
+      <c r="AA9" s="4">
+        <v>1</v>
+      </c>
       <c r="AB9" s="4"/>
       <c r="AC9" s="4"/>
-      <c r="AD9" s="4">
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="4">
         <v>2</v>
       </c>
-      <c r="AE9" s="9">
+      <c r="AH9" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1973</v>
       </c>
@@ -2030,28 +2066,28 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="4">
-        <v>1</v>
-      </c>
+      <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="J10" s="4">
+        <v>1</v>
+      </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="4">
-        <v>1</v>
-      </c>
+      <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4">
+        <v>1</v>
+      </c>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4">
         <v>3</v>
       </c>
-      <c r="R10" s="4">
+      <c r="U10" s="4">
         <v>2</v>
       </c>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
@@ -2061,12 +2097,15 @@
       <c r="AB10" s="4"/>
       <c r="AC10" s="4"/>
       <c r="AD10" s="4"/>
-      <c r="AE10" s="9">
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="4"/>
+      <c r="AH10" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1974</v>
       </c>
@@ -2082,37 +2121,40 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
-      <c r="N11" s="4">
-        <v>1</v>
-      </c>
+      <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-      <c r="P11" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4">
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4">
+        <v>1</v>
+      </c>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4">
+        <v>1</v>
+      </c>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4">
         <v>2</v>
       </c>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
-      <c r="X11" s="4">
-        <v>3</v>
-      </c>
+      <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
-      <c r="AA11" s="4"/>
+      <c r="AA11" s="4">
+        <v>3</v>
+      </c>
       <c r="AB11" s="4"/>
       <c r="AC11" s="4"/>
       <c r="AD11" s="4"/>
-      <c r="AE11" s="9">
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4"/>
+      <c r="AG11" s="4"/>
+      <c r="AH11" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>1975</v>
       </c>
@@ -2122,43 +2164,46 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="4">
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4">
         <v>2</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="4">
-        <v>1</v>
-      </c>
+      <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4">
+        <v>1</v>
+      </c>
       <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
+      <c r="S12" s="4">
+        <v>1</v>
+      </c>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
-      <c r="X12" s="4">
-        <v>3</v>
-      </c>
+      <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
+      <c r="AA12" s="4">
+        <v>3</v>
+      </c>
       <c r="AB12" s="4"/>
       <c r="AC12" s="4"/>
       <c r="AD12" s="4"/>
-      <c r="AE12" s="9">
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="4"/>
+      <c r="AH12" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>1976</v>
       </c>
@@ -2174,37 +2219,40 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="4">
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4">
         <v>3</v>
       </c>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4">
+      <c r="R13" s="4"/>
+      <c r="S13" s="4">
+        <v>1</v>
+      </c>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4">
         <v>2</v>
       </c>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
-      <c r="X13" s="4">
-        <v>1</v>
-      </c>
+      <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
       <c r="Z13" s="4"/>
-      <c r="AA13" s="4"/>
+      <c r="AA13" s="4">
+        <v>1</v>
+      </c>
       <c r="AB13" s="4"/>
       <c r="AC13" s="4"/>
       <c r="AD13" s="4"/>
-      <c r="AE13" s="9">
+      <c r="AE13" s="4"/>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="4"/>
+      <c r="AH13" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>1977</v>
       </c>
@@ -2214,28 +2262,28 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="4">
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4">
         <v>3</v>
       </c>
-      <c r="I14" s="4">
+      <c r="K14" s="4">
         <v>2</v>
       </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
-      <c r="N14" s="4">
-        <v>1</v>
-      </c>
+      <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4">
-        <v>1</v>
-      </c>
+      <c r="Q14" s="4">
+        <v>1</v>
+      </c>
+      <c r="R14" s="4"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
+      <c r="U14" s="4">
+        <v>1</v>
+      </c>
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
@@ -2245,12 +2293,15 @@
       <c r="AB14" s="4"/>
       <c r="AC14" s="4"/>
       <c r="AD14" s="4"/>
-      <c r="AE14" s="9">
+      <c r="AE14" s="4"/>
+      <c r="AF14" s="4"/>
+      <c r="AG14" s="4"/>
+      <c r="AH14" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>1978</v>
       </c>
@@ -2262,46 +2313,49 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="4">
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4">
         <v>2</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="4">
-        <v>1</v>
-      </c>
+      <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
+      <c r="S15" s="4">
+        <v>1</v>
+      </c>
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
-      <c r="X15" s="4">
-        <v>3</v>
-      </c>
+      <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
       <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
+      <c r="AA15" s="4">
+        <v>3</v>
+      </c>
       <c r="AB15" s="4"/>
-      <c r="AC15" s="4">
+      <c r="AC15" s="4"/>
+      <c r="AD15" s="4"/>
+      <c r="AE15" s="4"/>
+      <c r="AF15" s="4">
         <v>2</v>
       </c>
-      <c r="AD15" s="4"/>
-      <c r="AE15" s="9">
+      <c r="AG15" s="4"/>
+      <c r="AH15" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AF15" s="8" t="s">
+      <c r="AI15" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>1979</v>
       </c>
@@ -2319,40 +2373,43 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="4">
-        <v>2</v>
-      </c>
+      <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
+      <c r="S16" s="4">
+        <v>2</v>
+      </c>
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
-      <c r="W16" s="4">
-        <v>1</v>
-      </c>
-      <c r="X16" s="4">
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="4">
         <v>3</v>
       </c>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
-      <c r="AB16" s="4">
-        <v>1</v>
-      </c>
-      <c r="AC16" s="4">
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="4"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF16" s="4">
         <v>2</v>
       </c>
-      <c r="AD16" s="4"/>
-      <c r="AE16" s="9">
+      <c r="AG16" s="4"/>
+      <c r="AH16" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AF16" s="8" t="s">
+      <c r="AI16" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>1980</v>
       </c>
@@ -2362,99 +2419,105 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="4">
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4">
         <v>2</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
-      <c r="N17" s="4">
-        <v>4</v>
-      </c>
+      <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
+      <c r="Q17" s="4">
+        <v>4</v>
+      </c>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
-      <c r="W17" s="4">
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4">
         <v>2</v>
       </c>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4">
-        <v>1</v>
-      </c>
-      <c r="Z17" s="4"/>
       <c r="AA17" s="4"/>
-      <c r="AB17" s="4"/>
+      <c r="AB17" s="4">
+        <v>1</v>
+      </c>
       <c r="AC17" s="4"/>
       <c r="AD17" s="4"/>
-      <c r="AE17" s="9">
+      <c r="AE17" s="4"/>
+      <c r="AF17" s="4"/>
+      <c r="AG17" s="4"/>
+      <c r="AH17" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AF17" s="8" t="s">
+      <c r="AI17" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>1981</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4">
-        <v>2</v>
-      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
+      <c r="J18" s="4">
+        <v>1</v>
+      </c>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
-      <c r="O18" s="4">
-        <v>1</v>
-      </c>
+      <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
+      <c r="R18" s="4">
+        <v>1</v>
+      </c>
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
-      <c r="U18" s="4">
-        <v>1</v>
-      </c>
+      <c r="U18" s="4"/>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
+      <c r="X18" s="4">
+        <v>1</v>
+      </c>
       <c r="Y18" s="4"/>
-      <c r="Z18" s="4">
-        <v>3</v>
-      </c>
+      <c r="Z18" s="4"/>
       <c r="AA18" s="4"/>
       <c r="AB18" s="4"/>
-      <c r="AC18" s="4"/>
+      <c r="AC18" s="4">
+        <v>3</v>
+      </c>
       <c r="AD18" s="4"/>
-      <c r="AE18" s="9">
+      <c r="AE18" s="4"/>
+      <c r="AF18" s="4"/>
+      <c r="AG18" s="4"/>
+      <c r="AH18" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AF18" s="8" t="s">
+      <c r="AI18" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>1982</v>
       </c>
@@ -2464,54 +2527,57 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="4">
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4">
         <v>2</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4">
-        <v>1</v>
-      </c>
+      <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4">
-        <v>1</v>
-      </c>
-      <c r="O19" s="4">
-        <v>1</v>
-      </c>
+      <c r="M19" s="4">
+        <v>1</v>
+      </c>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4">
+        <v>1</v>
+      </c>
+      <c r="R19" s="4">
+        <v>1</v>
+      </c>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4">
         <v>3</v>
       </c>
-      <c r="R19" s="4">
-        <v>1</v>
-      </c>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4">
-        <v>2</v>
-      </c>
+      <c r="U19" s="4">
+        <v>1</v>
+      </c>
+      <c r="V19" s="4"/>
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
+      <c r="Y19" s="4">
+        <v>2</v>
+      </c>
       <c r="Z19" s="4"/>
       <c r="AA19" s="4"/>
       <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
-      <c r="AD19" s="4">
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="4"/>
+      <c r="AF19" s="4"/>
+      <c r="AG19" s="4">
         <v>4</v>
       </c>
-      <c r="AE19" s="9">
+      <c r="AH19" s="9">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="AF19" s="10" t="s">
+      <c r="AI19" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>1983</v>
       </c>
@@ -2527,53 +2593,56 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
-      <c r="N20" s="4">
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4">
         <v>3</v>
       </c>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
+      <c r="S20" s="4">
+        <v>1</v>
+      </c>
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
-      <c r="Z20" s="4">
-        <v>1</v>
-      </c>
-      <c r="AA20" s="4">
-        <v>2</v>
-      </c>
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="4"/>
       <c r="AB20" s="4"/>
-      <c r="AC20" s="4"/>
+      <c r="AC20" s="4">
+        <v>1</v>
+      </c>
       <c r="AD20" s="4">
         <v>2</v>
       </c>
-      <c r="AE20" s="9">
+      <c r="AE20" s="4"/>
+      <c r="AF20" s="4"/>
+      <c r="AG20" s="4">
+        <v>2</v>
+      </c>
+      <c r="AH20" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AF20" s="8" t="s">
+      <c r="AI20" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>1984</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="4">
-        <v>1</v>
-      </c>
+      <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="G21" s="4">
+        <v>1</v>
+      </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -2583,50 +2652,53 @@
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
-      <c r="Q21" s="4">
-        <v>2</v>
-      </c>
+      <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4">
-        <v>1</v>
-      </c>
+      <c r="T21" s="4">
+        <v>2</v>
+      </c>
+      <c r="U21" s="4"/>
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
       <c r="X21" s="4">
         <v>1</v>
       </c>
       <c r="Y21" s="4"/>
-      <c r="Z21" s="4">
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4">
         <v>3</v>
       </c>
-      <c r="AA21" s="4">
-        <v>1</v>
-      </c>
-      <c r="AB21" s="4"/>
-      <c r="AC21" s="4"/>
-      <c r="AD21" s="4"/>
-      <c r="AE21" s="9">
+      <c r="AD21" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE21" s="4"/>
+      <c r="AF21" s="4"/>
+      <c r="AG21" s="4"/>
+      <c r="AH21" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AF21" s="8" t="s">
+      <c r="AI21" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>1985</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="4">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4">
         <v>3</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -2635,38 +2707,41 @@
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
-      <c r="P22" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="4">
-        <v>1</v>
-      </c>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
       <c r="S22" s="4">
+        <v>1</v>
+      </c>
+      <c r="T22" s="4">
+        <v>1</v>
+      </c>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4">
         <v>3</v>
       </c>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4">
-        <v>1</v>
-      </c>
-      <c r="V22" s="4"/>
       <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
+      <c r="X22" s="4">
+        <v>1</v>
+      </c>
       <c r="Y22" s="4"/>
       <c r="Z22" s="4"/>
       <c r="AA22" s="4"/>
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
       <c r="AD22" s="4"/>
-      <c r="AE22" s="9">
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="4"/>
+      <c r="AG22" s="4"/>
+      <c r="AH22" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AF22" s="8" t="s">
+      <c r="AI22" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>1986</v>
       </c>
@@ -2675,15 +2750,15 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4">
-        <v>1</v>
-      </c>
+      <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4">
+        <v>1</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4">
         <v>2</v>
       </c>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -2693,31 +2768,34 @@
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
       <c r="T23" s="4"/>
-      <c r="U23" s="4">
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4">
         <v>3</v>
       </c>
-      <c r="V23" s="4">
-        <v>1</v>
-      </c>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
-      <c r="Y23" s="4"/>
+      <c r="Y23" s="4">
+        <v>1</v>
+      </c>
       <c r="Z23" s="4"/>
       <c r="AA23" s="4"/>
       <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
-      <c r="AD23" s="4">
+      <c r="AD23" s="4"/>
+      <c r="AE23" s="4"/>
+      <c r="AF23" s="4"/>
+      <c r="AG23" s="4">
         <v>2</v>
       </c>
-      <c r="AE23" s="9">
+      <c r="AH23" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AF23" s="8" t="s">
+      <c r="AI23" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>1987</v>
       </c>
@@ -2726,27 +2804,27 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="4">
-        <v>1</v>
-      </c>
+      <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4">
+        <v>1</v>
+      </c>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4">
         <v>2</v>
       </c>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
-      <c r="R24" s="4">
-        <v>2</v>
-      </c>
+      <c r="R24" s="4"/>
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
+      <c r="U24" s="4">
+        <v>2</v>
+      </c>
       <c r="V24" s="4"/>
       <c r="W24" s="4"/>
       <c r="X24" s="4"/>
@@ -2754,37 +2832,40 @@
       <c r="Z24" s="4"/>
       <c r="AA24" s="4"/>
       <c r="AB24" s="4"/>
-      <c r="AC24" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD24" s="4">
+      <c r="AC24" s="4"/>
+      <c r="AD24" s="4"/>
+      <c r="AE24" s="4"/>
+      <c r="AF24" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG24" s="4">
         <v>3</v>
       </c>
-      <c r="AE24" s="9">
+      <c r="AH24" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AF24" s="8" t="s">
+      <c r="AI24" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>1988</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="4">
-        <v>1</v>
-      </c>
+      <c r="D25" s="4"/>
       <c r="E25" s="4">
         <v>1</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="4"/>
+      <c r="G25" s="4">
+        <v>1</v>
+      </c>
+      <c r="H25" s="4">
         <v>2</v>
       </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -2794,34 +2875,37 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
-      <c r="R25" s="4">
-        <v>1</v>
-      </c>
+      <c r="R25" s="4"/>
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
+      <c r="U25" s="4">
+        <v>1</v>
+      </c>
       <c r="V25" s="4"/>
       <c r="W25" s="4"/>
       <c r="X25" s="4"/>
       <c r="Y25" s="4"/>
-      <c r="Z25" s="4">
-        <v>3</v>
-      </c>
+      <c r="Z25" s="4"/>
       <c r="AA25" s="4"/>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AD25" s="4"/>
-      <c r="AE25" s="9">
+      <c r="AE25" s="4"/>
+      <c r="AF25" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG25" s="4"/>
+      <c r="AH25" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AF25" s="8" t="s">
+      <c r="AI25" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>1989</v>
       </c>
@@ -2830,106 +2914,112 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="4">
-        <v>1</v>
-      </c>
+      <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4">
+        <v>1</v>
+      </c>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4">
         <v>2</v>
       </c>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
-      <c r="P26" s="4">
-        <v>2</v>
-      </c>
+      <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
+      <c r="S26" s="4">
+        <v>2</v>
+      </c>
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
       <c r="W26" s="4"/>
-      <c r="X26" s="4">
-        <v>1</v>
-      </c>
+      <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
-      <c r="Z26" s="4">
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="4">
         <v>3</v>
       </c>
-      <c r="AA26" s="4"/>
-      <c r="AB26" s="4"/>
-      <c r="AC26" s="4"/>
       <c r="AD26" s="4"/>
-      <c r="AE26" s="9">
+      <c r="AE26" s="4"/>
+      <c r="AF26" s="4"/>
+      <c r="AG26" s="4"/>
+      <c r="AH26" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AF26" s="8" t="s">
+      <c r="AI26" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>1990</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="4">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4">
         <v>2</v>
       </c>
-      <c r="E27" s="4">
-        <v>1</v>
-      </c>
-      <c r="F27" s="4">
-        <v>1</v>
-      </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4">
+        <v>1</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1</v>
+      </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
-      <c r="N27" s="4">
-        <v>1</v>
-      </c>
-      <c r="O27" s="11"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4">
         <v>1</v>
       </c>
-      <c r="R27" s="4"/>
+      <c r="R27" s="11"/>
       <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4">
-        <v>3</v>
-      </c>
+      <c r="T27" s="4">
+        <v>1</v>
+      </c>
+      <c r="U27" s="4"/>
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
-      <c r="X27" s="4"/>
+      <c r="X27" s="4">
+        <v>3</v>
+      </c>
       <c r="Y27" s="4"/>
-      <c r="Z27" s="4">
-        <v>1</v>
-      </c>
+      <c r="Z27" s="4"/>
       <c r="AA27" s="4"/>
       <c r="AB27" s="4"/>
-      <c r="AC27" s="4"/>
-      <c r="AD27" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE27" s="9">
+      <c r="AC27" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD27" s="4"/>
+      <c r="AE27" s="4"/>
+      <c r="AF27" s="4"/>
+      <c r="AG27" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH27" s="9">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="AF27" s="8" t="s">
+      <c r="AI27" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>1991</v>
       </c>
@@ -2937,31 +3027,31 @@
       <c r="C28" s="4">
         <v>1</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="4"/>
+      <c r="E28" s="4">
         <v>2</v>
       </c>
-      <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="4">
-        <v>1</v>
-      </c>
-      <c r="I28" s="4">
-        <v>1</v>
-      </c>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
       <c r="J28" s="4">
         <v>1</v>
       </c>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4">
-        <v>1</v>
-      </c>
+      <c r="K28" s="4">
+        <v>1</v>
+      </c>
+      <c r="L28" s="4">
+        <v>1</v>
+      </c>
+      <c r="M28" s="4"/>
       <c r="N28" s="4"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4">
+        <v>1</v>
+      </c>
       <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
+      <c r="R28" s="11"/>
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
@@ -2972,398 +3062,606 @@
       <c r="Z28" s="4"/>
       <c r="AA28" s="4"/>
       <c r="AB28" s="4"/>
-      <c r="AC28" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD28" s="4">
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="4"/>
+      <c r="AE28" s="4"/>
+      <c r="AF28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG28" s="4">
         <v>3</v>
       </c>
-      <c r="AE28" s="9">
+      <c r="AH28" s="9">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="AI28" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
         <v>1992</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
-      <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
-      <c r="X29" s="2"/>
-      <c r="Y29" s="2"/>
-      <c r="Z29" s="2"/>
-      <c r="AA29" s="2"/>
-      <c r="AB29" s="2"/>
-      <c r="AC29" s="2"/>
-      <c r="AD29" s="2"/>
-      <c r="AE29" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4">
+        <v>3</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4">
+        <v>3</v>
+      </c>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4">
+        <v>1</v>
+      </c>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC29" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD29" s="4"/>
+      <c r="AE29" s="4"/>
+      <c r="AF29" s="4"/>
+      <c r="AG29" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH29" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AI29" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
         <v>1993</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
-      <c r="T30" s="2"/>
-      <c r="U30" s="2"/>
-      <c r="V30" s="2"/>
-      <c r="W30" s="2"/>
-      <c r="X30" s="2"/>
-      <c r="Y30" s="2"/>
-      <c r="Z30" s="2"/>
-      <c r="AA30" s="2"/>
-      <c r="AB30" s="2"/>
-      <c r="AC30" s="2"/>
-      <c r="AD30" s="2"/>
-      <c r="AE30" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4">
+        <v>2</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4">
+        <v>3</v>
+      </c>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4">
+        <v>1</v>
+      </c>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>1</v>
+      </c>
+      <c r="R30" s="11"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4"/>
+      <c r="AB30" s="4"/>
+      <c r="AC30" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD30" s="4"/>
+      <c r="AE30" s="4"/>
+      <c r="AF30" s="4"/>
+      <c r="AG30" s="4"/>
+      <c r="AH30" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AI30" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
         <v>1994</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
-      <c r="W31" s="2"/>
-      <c r="X31" s="2"/>
-      <c r="Y31" s="2"/>
-      <c r="Z31" s="2"/>
-      <c r="AA31" s="2"/>
-      <c r="AB31" s="2"/>
-      <c r="AC31" s="2"/>
-      <c r="AD31" s="2"/>
-      <c r="AE31" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4">
+        <v>1</v>
+      </c>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4">
+        <v>1</v>
+      </c>
+      <c r="J31" s="4">
+        <v>1</v>
+      </c>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4">
+        <v>1</v>
+      </c>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4">
+        <v>1</v>
+      </c>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB31" s="4">
+        <v>2</v>
+      </c>
+      <c r="AC31" s="4">
+        <v>3</v>
+      </c>
+      <c r="AD31" s="4"/>
+      <c r="AE31" s="4"/>
+      <c r="AF31" s="4"/>
+      <c r="AG31" s="4"/>
+      <c r="AH31" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AI31" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
         <v>1995</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
-      <c r="U32" s="2"/>
-      <c r="V32" s="2"/>
-      <c r="W32" s="2"/>
-      <c r="X32" s="2"/>
-      <c r="Y32" s="2"/>
-      <c r="Z32" s="2"/>
-      <c r="AA32" s="2"/>
-      <c r="AB32" s="2"/>
-      <c r="AC32" s="2"/>
-      <c r="AD32" s="2"/>
-      <c r="AE32" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4">
+        <v>1</v>
+      </c>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4">
+        <v>3</v>
+      </c>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4">
+        <v>2</v>
+      </c>
+      <c r="N32" s="4">
+        <v>2</v>
+      </c>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
+      <c r="Y32" s="4"/>
+      <c r="Z32" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA32" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB32" s="4"/>
+      <c r="AC32" s="4"/>
+      <c r="AD32" s="4"/>
+      <c r="AE32" s="4"/>
+      <c r="AF32" s="4"/>
+      <c r="AG32" s="4"/>
+      <c r="AH32" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AI32" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
         <v>1996</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
-      <c r="V33" s="2"/>
-      <c r="W33" s="2"/>
-      <c r="X33" s="2"/>
-      <c r="Y33" s="2"/>
-      <c r="Z33" s="2"/>
-      <c r="AA33" s="2"/>
-      <c r="AB33" s="2"/>
-      <c r="AC33" s="2"/>
-      <c r="AD33" s="2"/>
-      <c r="AE33" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4">
+        <v>1</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4">
+        <v>1</v>
+      </c>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4">
+        <v>3</v>
+      </c>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4">
+        <v>2</v>
+      </c>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4">
+        <v>2</v>
+      </c>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
+      <c r="AA33" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB33" s="4"/>
+      <c r="AC33" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD33" s="4"/>
+      <c r="AE33" s="4"/>
+      <c r="AF33" s="4"/>
+      <c r="AG33" s="4"/>
+      <c r="AH33" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AI33" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
         <v>1997</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
-      <c r="U34" s="2"/>
-      <c r="V34" s="2"/>
-      <c r="W34" s="2"/>
-      <c r="X34" s="2"/>
-      <c r="Y34" s="2"/>
-      <c r="Z34" s="2"/>
-      <c r="AA34" s="2"/>
-      <c r="AB34" s="2"/>
-      <c r="AC34" s="2"/>
-      <c r="AD34" s="2"/>
-      <c r="AE34" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4">
+        <v>4</v>
+      </c>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4">
+        <v>2</v>
+      </c>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4">
+        <v>1</v>
+      </c>
+      <c r="V34" s="4">
+        <v>1</v>
+      </c>
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="4"/>
+      <c r="AA34" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB34" s="4"/>
+      <c r="AC34" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD34" s="4"/>
+      <c r="AE34" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF34" s="4"/>
+      <c r="AG34" s="4"/>
+      <c r="AH34" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AI34" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
         <v>1998</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
-      <c r="V35" s="2"/>
-      <c r="W35" s="2"/>
-      <c r="X35" s="2"/>
-      <c r="Y35" s="2"/>
-      <c r="Z35" s="2"/>
-      <c r="AA35" s="2"/>
-      <c r="AB35" s="2"/>
-      <c r="AC35" s="2"/>
-      <c r="AD35" s="2"/>
-      <c r="AE35" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="B35" s="4">
+        <v>1</v>
+      </c>
+      <c r="C35" s="4">
+        <v>2</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4">
+        <v>3</v>
+      </c>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4">
+        <v>1</v>
+      </c>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4">
+        <v>1</v>
+      </c>
+      <c r="U35" s="4">
+        <v>1</v>
+      </c>
+      <c r="V35" s="4"/>
+      <c r="W35" s="4"/>
+      <c r="X35" s="4"/>
+      <c r="Y35" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z35" s="4"/>
+      <c r="AA35" s="4"/>
+      <c r="AB35" s="4"/>
+      <c r="AC35" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD35" s="4"/>
+      <c r="AE35" s="4"/>
+      <c r="AF35" s="4"/>
+      <c r="AG35" s="4"/>
+      <c r="AH35" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AI35" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
         <v>1999</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
-      <c r="U36" s="2"/>
-      <c r="V36" s="2"/>
-      <c r="W36" s="2"/>
-      <c r="X36" s="2"/>
-      <c r="Y36" s="2"/>
-      <c r="Z36" s="2"/>
-      <c r="AA36" s="2"/>
-      <c r="AB36" s="2"/>
-      <c r="AC36" s="2"/>
-      <c r="AD36" s="2"/>
-      <c r="AE36" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4">
+        <v>1</v>
+      </c>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="4">
+        <v>3</v>
+      </c>
+      <c r="T36" s="4">
+        <v>1</v>
+      </c>
+      <c r="U36" s="4">
+        <v>1</v>
+      </c>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+      <c r="Z36" s="4"/>
+      <c r="AA36" s="4"/>
+      <c r="AB36" s="4"/>
+      <c r="AC36" s="4"/>
+      <c r="AD36" s="4"/>
+      <c r="AE36" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF36" s="4">
+        <v>3</v>
+      </c>
+      <c r="AG36" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH36" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AI36" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
         <v>2000</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="2"/>
-      <c r="Q37" s="2"/>
-      <c r="R37" s="2"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="2"/>
-      <c r="U37" s="2"/>
-      <c r="V37" s="2"/>
-      <c r="W37" s="2"/>
-      <c r="X37" s="2"/>
-      <c r="Y37" s="2"/>
-      <c r="Z37" s="2"/>
-      <c r="AA37" s="2"/>
-      <c r="AB37" s="2"/>
-      <c r="AC37" s="2"/>
-      <c r="AD37" s="2"/>
-      <c r="AE37" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4">
+        <v>4</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4">
+        <v>1</v>
+      </c>
+      <c r="R37" s="11"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4">
+        <v>1</v>
+      </c>
+      <c r="U37" s="4">
+        <v>1</v>
+      </c>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4">
+        <v>1</v>
+      </c>
+      <c r="X37" s="4">
+        <v>2</v>
+      </c>
+      <c r="Y37" s="4"/>
+      <c r="Z37" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA37" s="4"/>
+      <c r="AB37" s="4"/>
+      <c r="AC37" s="4"/>
+      <c r="AD37" s="4"/>
+      <c r="AE37" s="4"/>
+      <c r="AF37" s="4"/>
+      <c r="AG37" s="4"/>
+      <c r="AH37" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AI37" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
         <v>2001</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="2"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="2"/>
-      <c r="U38" s="2"/>
-      <c r="V38" s="2"/>
-      <c r="W38" s="2"/>
-      <c r="X38" s="2"/>
-      <c r="Y38" s="2"/>
-      <c r="Z38" s="2"/>
-      <c r="AA38" s="2"/>
-      <c r="AB38" s="2"/>
-      <c r="AC38" s="2"/>
-      <c r="AD38" s="2"/>
-      <c r="AE38" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4">
+        <v>1</v>
+      </c>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4">
+        <v>1</v>
+      </c>
+      <c r="R38" s="11"/>
+      <c r="S38" s="4">
+        <v>2</v>
+      </c>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4">
+        <v>3</v>
+      </c>
+      <c r="W38" s="4"/>
+      <c r="X38" s="4"/>
+      <c r="Y38" s="4"/>
+      <c r="Z38" s="4">
+        <v>2</v>
+      </c>
+      <c r="AA38" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB38" s="4"/>
+      <c r="AC38" s="4"/>
+      <c r="AD38" s="4"/>
+      <c r="AE38" s="4"/>
+      <c r="AF38" s="4"/>
+      <c r="AG38" s="4"/>
+      <c r="AH38" s="9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AI38" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>2002</v>
       </c>
@@ -3380,10 +3678,10 @@
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
-      <c r="O39" s="6"/>
+      <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
+      <c r="R39" s="6"/>
       <c r="S39" s="2"/>
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
@@ -3396,12 +3694,18 @@
       <c r="AB39" s="2"/>
       <c r="AC39" s="2"/>
       <c r="AD39" s="2"/>
-      <c r="AE39" s="9">
+      <c r="AE39" s="2"/>
+      <c r="AF39" s="2"/>
+      <c r="AG39" s="2"/>
+      <c r="AH39" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI39" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>2003</v>
       </c>
@@ -3418,10 +3722,10 @@
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
-      <c r="O40" s="6"/>
+      <c r="O40" s="2"/>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
+      <c r="R40" s="6"/>
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
@@ -3434,12 +3738,18 @@
       <c r="AB40" s="2"/>
       <c r="AC40" s="2"/>
       <c r="AD40" s="2"/>
-      <c r="AE40" s="9">
+      <c r="AE40" s="2"/>
+      <c r="AF40" s="2"/>
+      <c r="AG40" s="2"/>
+      <c r="AH40" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI40" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>2004</v>
       </c>
@@ -3456,10 +3766,10 @@
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
-      <c r="O41" s="6"/>
+      <c r="O41" s="2"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
-      <c r="R41" s="2"/>
+      <c r="R41" s="6"/>
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
@@ -3472,12 +3782,18 @@
       <c r="AB41" s="2"/>
       <c r="AC41" s="2"/>
       <c r="AD41" s="2"/>
-      <c r="AE41" s="9">
+      <c r="AE41" s="2"/>
+      <c r="AF41" s="2"/>
+      <c r="AG41" s="2"/>
+      <c r="AH41" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI41" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>2005</v>
       </c>
@@ -3494,10 +3810,10 @@
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
-      <c r="O42" s="6"/>
+      <c r="O42" s="2"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
-      <c r="R42" s="2"/>
+      <c r="R42" s="6"/>
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
@@ -3509,15 +3825,19 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
       <c r="AC42" s="2"/>
-      <c r="AD42" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE42" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AD42" s="2"/>
+      <c r="AE42" s="2"/>
+      <c r="AF42" s="2"/>
+      <c r="AG42" s="2"/>
+      <c r="AH42" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AI42" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>2006</v>
       </c>
@@ -3534,10 +3854,10 @@
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
-      <c r="O43" s="6"/>
+      <c r="O43" s="2"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
-      <c r="R43" s="2"/>
+      <c r="R43" s="6"/>
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
@@ -3550,12 +3870,18 @@
       <c r="AB43" s="2"/>
       <c r="AC43" s="2"/>
       <c r="AD43" s="2"/>
-      <c r="AE43" s="9">
+      <c r="AE43" s="2"/>
+      <c r="AF43" s="2"/>
+      <c r="AG43" s="2"/>
+      <c r="AH43" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI43" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>2007</v>
       </c>
@@ -3572,10 +3898,10 @@
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
-      <c r="O44" s="6"/>
+      <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
-      <c r="R44" s="2"/>
+      <c r="R44" s="6"/>
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
@@ -3587,15 +3913,19 @@
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
       <c r="AC44" s="2"/>
-      <c r="AD44" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE44" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AD44" s="2"/>
+      <c r="AE44" s="2"/>
+      <c r="AF44" s="2"/>
+      <c r="AG44" s="2"/>
+      <c r="AH44" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AI44" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>2008</v>
       </c>
@@ -3612,10 +3942,10 @@
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
-      <c r="O45" s="6"/>
+      <c r="O45" s="2"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
-      <c r="R45" s="2"/>
+      <c r="R45" s="6"/>
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
@@ -3628,12 +3958,18 @@
       <c r="AB45" s="2"/>
       <c r="AC45" s="2"/>
       <c r="AD45" s="2"/>
-      <c r="AE45" s="9">
+      <c r="AE45" s="2"/>
+      <c r="AF45" s="2"/>
+      <c r="AG45" s="2"/>
+      <c r="AH45" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI45" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>2009</v>
       </c>
@@ -3650,10 +3986,10 @@
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
-      <c r="O46" s="6"/>
+      <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
-      <c r="R46" s="2"/>
+      <c r="R46" s="6"/>
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
@@ -3666,12 +4002,18 @@
       <c r="AB46" s="2"/>
       <c r="AC46" s="2"/>
       <c r="AD46" s="2"/>
-      <c r="AE46" s="9">
+      <c r="AE46" s="2"/>
+      <c r="AF46" s="2"/>
+      <c r="AG46" s="2"/>
+      <c r="AH46" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI46" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>2010</v>
       </c>
@@ -3688,10 +4030,10 @@
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
-      <c r="O47" s="6"/>
+      <c r="O47" s="2"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
-      <c r="R47" s="2"/>
+      <c r="R47" s="6"/>
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
@@ -3704,12 +4046,18 @@
       <c r="AB47" s="2"/>
       <c r="AC47" s="2"/>
       <c r="AD47" s="2"/>
-      <c r="AE47" s="9">
+      <c r="AE47" s="2"/>
+      <c r="AF47" s="2"/>
+      <c r="AG47" s="2"/>
+      <c r="AH47" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI47" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>2011</v>
       </c>
@@ -3726,10 +4074,10 @@
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
-      <c r="O48" s="6"/>
+      <c r="O48" s="2"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
-      <c r="R48" s="2"/>
+      <c r="R48" s="6"/>
       <c r="S48" s="2"/>
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
@@ -3742,12 +4090,18 @@
       <c r="AB48" s="2"/>
       <c r="AC48" s="2"/>
       <c r="AD48" s="2"/>
-      <c r="AE48" s="9">
+      <c r="AE48" s="2"/>
+      <c r="AF48" s="2"/>
+      <c r="AG48" s="2"/>
+      <c r="AH48" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI48" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>2012</v>
       </c>
@@ -3764,10 +4118,10 @@
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
-      <c r="O49" s="6"/>
+      <c r="O49" s="2"/>
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
+      <c r="R49" s="6"/>
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
@@ -3779,15 +4133,19 @@
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
       <c r="AC49" s="2"/>
-      <c r="AD49" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE49" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AD49" s="2"/>
+      <c r="AE49" s="2"/>
+      <c r="AF49" s="2"/>
+      <c r="AG49" s="2"/>
+      <c r="AH49" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AI49" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>2013</v>
       </c>
@@ -3804,10 +4162,10 @@
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
-      <c r="O50" s="6"/>
+      <c r="O50" s="2"/>
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
-      <c r="R50" s="2"/>
+      <c r="R50" s="6"/>
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
@@ -3820,12 +4178,18 @@
       <c r="AB50" s="2"/>
       <c r="AC50" s="2"/>
       <c r="AD50" s="2"/>
-      <c r="AE50" s="9">
+      <c r="AE50" s="2"/>
+      <c r="AF50" s="2"/>
+      <c r="AG50" s="2"/>
+      <c r="AH50" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AI50" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>2014</v>
       </c>
@@ -3842,10 +4206,10 @@
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
-      <c r="O51" s="6"/>
+      <c r="O51" s="2"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
-      <c r="R51" s="2"/>
+      <c r="R51" s="6"/>
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
@@ -3858,12 +4222,15 @@
       <c r="AB51" s="2"/>
       <c r="AC51" s="2"/>
       <c r="AD51" s="2"/>
-      <c r="AE51" s="9">
+      <c r="AE51" s="2"/>
+      <c r="AF51" s="2"/>
+      <c r="AG51" s="2"/>
+      <c r="AH51" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>2015</v>
       </c>
@@ -3895,15 +4262,16 @@
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
       <c r="AC52" s="2"/>
-      <c r="AD52" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE52" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AD52" s="2"/>
+      <c r="AE52" s="2"/>
+      <c r="AF52" s="2"/>
+      <c r="AG52" s="2"/>
+      <c r="AH52" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>2016</v>
       </c>
@@ -3920,10 +4288,10 @@
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
-      <c r="O53" s="7"/>
+      <c r="O53" s="2"/>
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
-      <c r="R53" s="2"/>
+      <c r="R53" s="7"/>
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
@@ -3936,12 +4304,15 @@
       <c r="AB53" s="2"/>
       <c r="AC53" s="2"/>
       <c r="AD53" s="2"/>
-      <c r="AE53" s="9">
+      <c r="AE53" s="2"/>
+      <c r="AF53" s="2"/>
+      <c r="AG53" s="2"/>
+      <c r="AH53" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>2017</v>
       </c>
@@ -3958,10 +4329,10 @@
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
-      <c r="O54" s="7"/>
+      <c r="O54" s="2"/>
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
-      <c r="R54" s="2"/>
+      <c r="R54" s="7"/>
       <c r="S54" s="2"/>
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
@@ -3974,12 +4345,15 @@
       <c r="AB54" s="2"/>
       <c r="AC54" s="2"/>
       <c r="AD54" s="2"/>
-      <c r="AE54" s="9">
+      <c r="AE54" s="2"/>
+      <c r="AF54" s="2"/>
+      <c r="AG54" s="2"/>
+      <c r="AH54" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>2018</v>
       </c>
@@ -3996,10 +4370,10 @@
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
-      <c r="O55" s="7"/>
+      <c r="O55" s="2"/>
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
-      <c r="R55" s="2"/>
+      <c r="R55" s="7"/>
       <c r="S55" s="2"/>
       <c r="T55" s="2"/>
       <c r="U55" s="2"/>
@@ -4012,12 +4386,15 @@
       <c r="AB55" s="2"/>
       <c r="AC55" s="2"/>
       <c r="AD55" s="2"/>
-      <c r="AE55" s="9">
+      <c r="AE55" s="2"/>
+      <c r="AF55" s="2"/>
+      <c r="AG55" s="2"/>
+      <c r="AH55" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>2019</v>
       </c>
@@ -4034,10 +4411,10 @@
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
-      <c r="O56" s="7"/>
+      <c r="O56" s="2"/>
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
-      <c r="R56" s="2"/>
+      <c r="R56" s="7"/>
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
@@ -4050,12 +4427,15 @@
       <c r="AB56" s="2"/>
       <c r="AC56" s="2"/>
       <c r="AD56" s="2"/>
-      <c r="AE56" s="9">
+      <c r="AE56" s="2"/>
+      <c r="AF56" s="2"/>
+      <c r="AG56" s="2"/>
+      <c r="AH56" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>2020</v>
       </c>
@@ -4072,10 +4452,10 @@
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
-      <c r="O57" s="7"/>
+      <c r="O57" s="2"/>
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
-      <c r="R57" s="2"/>
+      <c r="R57" s="7"/>
       <c r="S57" s="2"/>
       <c r="T57" s="2"/>
       <c r="U57" s="2"/>
@@ -4087,15 +4467,16 @@
       <c r="AA57" s="2"/>
       <c r="AB57" s="2"/>
       <c r="AC57" s="2"/>
-      <c r="AD57" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE57" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AD57" s="2"/>
+      <c r="AE57" s="2"/>
+      <c r="AF57" s="2"/>
+      <c r="AG57" s="2"/>
+      <c r="AH57" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>2021</v>
       </c>
@@ -4112,10 +4493,10 @@
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
-      <c r="O58" s="7"/>
+      <c r="O58" s="2"/>
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
-      <c r="R58" s="2"/>
+      <c r="R58" s="7"/>
       <c r="S58" s="2"/>
       <c r="T58" s="2"/>
       <c r="U58" s="2"/>
@@ -4128,12 +4509,15 @@
       <c r="AB58" s="2"/>
       <c r="AC58" s="2"/>
       <c r="AD58" s="2"/>
-      <c r="AE58" s="9">
+      <c r="AE58" s="2"/>
+      <c r="AF58" s="2"/>
+      <c r="AG58" s="2"/>
+      <c r="AH58" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>2022</v>
       </c>
@@ -4150,10 +4534,10 @@
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
-      <c r="O59" s="7"/>
+      <c r="O59" s="2"/>
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
-      <c r="R59" s="2"/>
+      <c r="R59" s="7"/>
       <c r="S59" s="2"/>
       <c r="T59" s="2"/>
       <c r="U59" s="2"/>
@@ -4166,94 +4550,97 @@
       <c r="AB59" s="2"/>
       <c r="AC59" s="2"/>
       <c r="AD59" s="2"/>
-      <c r="AE59" s="9">
+      <c r="AE59" s="2"/>
+      <c r="AF59" s="2"/>
+      <c r="AG59" s="2"/>
+      <c r="AH59" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O60" s="1"/>
-    </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O61" s="1"/>
-    </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O62" s="1"/>
-    </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O63" s="1"/>
-    </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="O64" s="1"/>
-    </row>
-    <row r="65" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O65" s="1"/>
-    </row>
-    <row r="66" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O66" s="1"/>
-    </row>
-    <row r="67" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O67" s="1"/>
-    </row>
-    <row r="68" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O68" s="1"/>
-    </row>
-    <row r="69" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O69" s="1"/>
-    </row>
-    <row r="70" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O70" s="1"/>
-    </row>
-    <row r="71" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O71" s="1"/>
-    </row>
-    <row r="72" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O72" s="1"/>
-    </row>
-    <row r="73" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O73" s="1"/>
-    </row>
-    <row r="74" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O74" s="1"/>
-    </row>
-    <row r="75" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O75" s="1"/>
-    </row>
-    <row r="76" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O76" s="1"/>
-    </row>
-    <row r="77" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O77" s="1"/>
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="R60" s="1"/>
+    </row>
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="R61" s="1"/>
+    </row>
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="R62" s="1"/>
+    </row>
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="R63" s="1"/>
+    </row>
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="R64" s="1"/>
+    </row>
+    <row r="65" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R65" s="1"/>
+    </row>
+    <row r="66" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R66" s="1"/>
+    </row>
+    <row r="67" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R67" s="1"/>
+    </row>
+    <row r="68" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R68" s="1"/>
+    </row>
+    <row r="69" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R69" s="1"/>
+    </row>
+    <row r="70" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R70" s="1"/>
+    </row>
+    <row r="71" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R71" s="1"/>
+    </row>
+    <row r="72" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R72" s="1"/>
+    </row>
+    <row r="73" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R73" s="1"/>
+    </row>
+    <row r="74" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R74" s="1"/>
+    </row>
+    <row r="75" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R75" s="1"/>
+    </row>
+    <row r="76" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R76" s="1"/>
+    </row>
+    <row r="77" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R77" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="O1:O76">
-    <sortCondition ref="O1"/>
+  <sortState ref="R1:R76">
+    <sortCondition ref="R1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1" display="https://www.nfl.com/teams/las-vegas-raiders/"/>
-    <hyperlink ref="L3" r:id="rId2" display="https://www.nfl.com/teams/indianapolis-colts/"/>
-    <hyperlink ref="P3" r:id="rId3" display="https://www.nfl.com/teams/los-angeles-rams/"/>
-    <hyperlink ref="K3" r:id="rId4" display="https://www.nfl.com/teams/green-bay-packers/"/>
-    <hyperlink ref="AC3" r:id="rId5" display="https://www.nfl.com/teams/tennessee-titans/"/>
-    <hyperlink ref="G3" r:id="rId6" display="https://www.nfl.com/teams/cleveland-browns/"/>
-    <hyperlink ref="H3" r:id="rId7" display="https://www.nfl.com/teams/dallas-cowboys/"/>
-    <hyperlink ref="M3" r:id="rId8" display="https://www.nfl.com/teams/kansas-city-chiefs/"/>
-    <hyperlink ref="O3" r:id="rId9" display="https://www.nfl.com/teams/los-angeles-chargers/"/>
-    <hyperlink ref="V3" r:id="rId10" display="https://www.nfl.com/teams/new-york-jets/"/>
-    <hyperlink ref="E3" r:id="rId11" display="https://www.nfl.com/teams/chicago-bears/"/>
-    <hyperlink ref="U3" r:id="rId12" display="https://www.nfl.com/teams/new-york-giants/"/>
-    <hyperlink ref="Z3" r:id="rId13" display="https://www.nfl.com/teams/san-francisco-49ers/"/>
+    <hyperlink ref="Q3" r:id="rId1" display="https://www.nfl.com/teams/las-vegas-raiders/"/>
+    <hyperlink ref="N3" r:id="rId2" display="https://www.nfl.com/teams/indianapolis-colts/"/>
+    <hyperlink ref="S3" r:id="rId3" display="https://www.nfl.com/teams/los-angeles-rams/"/>
+    <hyperlink ref="M3" r:id="rId4" display="https://www.nfl.com/teams/green-bay-packers/"/>
+    <hyperlink ref="AF3" r:id="rId5" display="https://www.nfl.com/teams/tennessee-titans/"/>
+    <hyperlink ref="I3" r:id="rId6" display="https://www.nfl.com/teams/cleveland-browns/"/>
+    <hyperlink ref="J3" r:id="rId7" display="https://www.nfl.com/teams/dallas-cowboys/"/>
+    <hyperlink ref="P3" r:id="rId8" display="https://www.nfl.com/teams/kansas-city-chiefs/"/>
+    <hyperlink ref="R3" r:id="rId9" display="https://www.nfl.com/teams/los-angeles-chargers/"/>
+    <hyperlink ref="Y3" r:id="rId10" display="https://www.nfl.com/teams/new-york-jets/"/>
+    <hyperlink ref="G3" r:id="rId11" display="https://www.nfl.com/teams/chicago-bears/"/>
+    <hyperlink ref="X3" r:id="rId12" display="https://www.nfl.com/teams/new-york-giants/"/>
+    <hyperlink ref="AC3" r:id="rId13" display="https://www.nfl.com/teams/san-francisco-49ers/"/>
     <hyperlink ref="B3" r:id="rId14" display="https://www.nfl.com/teams/arizona-cardinals/"/>
-    <hyperlink ref="W3" r:id="rId15" display="https://www.nfl.com/teams/philadelphia-eagles/"/>
-    <hyperlink ref="AD3" r:id="rId16" display="https://www.nfl.com/teams/washington-commanders/"/>
-    <hyperlink ref="J3" r:id="rId17" display="https://www.nfl.com/teams/detroit-lions/"/>
-    <hyperlink ref="X3" r:id="rId18" display="https://www.nfl.com/teams/pittsburgh-steelers/"/>
-    <hyperlink ref="D3" r:id="rId19" display="https://www.nfl.com/teams/buffalo-bills/"/>
-    <hyperlink ref="Q3" r:id="rId20" display="https://www.nfl.com/teams/miami-dolphins/"/>
-    <hyperlink ref="R3" r:id="rId21" display="https://www.nfl.com/teams/minnesota-vikings/"/>
-    <hyperlink ref="S3" r:id="rId22" display="https://www.nfl.com/teams/new-england-patriots/"/>
-    <hyperlink ref="I3" r:id="rId23" display="https://www.nfl.com/teams/denver-broncos/"/>
-    <hyperlink ref="T3" r:id="rId24" display="https://www.nfl.com/teams/new-orleans-saints/"/>
+    <hyperlink ref="Z3" r:id="rId15" display="https://www.nfl.com/teams/philadelphia-eagles/"/>
+    <hyperlink ref="AG3" r:id="rId16" display="https://www.nfl.com/teams/washington-commanders/"/>
+    <hyperlink ref="L3" r:id="rId17" display="https://www.nfl.com/teams/detroit-lions/"/>
+    <hyperlink ref="AA3" r:id="rId18" display="https://www.nfl.com/teams/pittsburgh-steelers/"/>
+    <hyperlink ref="E3" r:id="rId19" display="https://www.nfl.com/teams/buffalo-bills/"/>
+    <hyperlink ref="T3" r:id="rId20" display="https://www.nfl.com/teams/miami-dolphins/"/>
+    <hyperlink ref="U3" r:id="rId21" display="https://www.nfl.com/teams/minnesota-vikings/"/>
+    <hyperlink ref="V3" r:id="rId22" display="https://www.nfl.com/teams/new-england-patriots/"/>
+    <hyperlink ref="K3" r:id="rId23" display="https://www.nfl.com/teams/denver-broncos/"/>
+    <hyperlink ref="W3" r:id="rId24" display="https://www.nfl.com/teams/new-orleans-saints/"/>
     <hyperlink ref="C3" r:id="rId25" display="https://www.nfl.com/teams/atlanta-falcons/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Populated all playoff data through 2021!
</commit_message>
<xml_diff>
--- a/NFL_playoff_wins.xlsx
+++ b/NFL_playoff_wins.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
   <si>
     <t>Year</t>
   </si>
@@ -142,6 +142,12 @@
   <si>
     <t>Baltimore Ravens</t>
   </si>
+  <si>
+    <t>Houston Texans</t>
+  </si>
+  <si>
+    <t>6 Wildcard games</t>
+  </si>
 </sst>
 </file>
 
@@ -229,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -240,18 +246,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -276,13 +279,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -320,13 +323,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -364,13 +367,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -408,13 +411,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -452,13 +455,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -496,13 +499,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -540,13 +543,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -584,15 +587,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -628,15 +631,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -672,15 +675,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -716,15 +719,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -760,15 +763,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -804,15 +807,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -848,15 +851,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -892,15 +895,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -936,15 +939,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -980,15 +983,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1024,15 +1027,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1068,15 +1071,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1112,15 +1115,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1156,15 +1159,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1200,15 +1203,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1244,15 +1247,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1288,15 +1291,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1332,15 +1335,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1640,30 +1643,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI77"/>
+  <dimension ref="A1:AJ76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T45" sqref="T45"/>
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="25" width="10.140625" customWidth="1"/>
-    <col min="26" max="26" width="15.5703125" customWidth="1"/>
-    <col min="27" max="28" width="10.140625" customWidth="1"/>
-    <col min="29" max="31" width="15.85546875" customWidth="1"/>
-    <col min="32" max="32" width="10.140625" customWidth="1"/>
-    <col min="33" max="33" width="14.85546875" customWidth="1"/>
-    <col min="35" max="35" width="21.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="10.140625" style="8"/>
+    <col min="2" max="26" width="10.140625" customWidth="1"/>
+    <col min="27" max="27" width="15.5703125" customWidth="1"/>
+    <col min="28" max="29" width="10.140625" customWidth="1"/>
+    <col min="30" max="32" width="15.85546875" customWidth="1"/>
+    <col min="33" max="33" width="10.140625" customWidth="1"/>
+    <col min="34" max="34" width="14.85546875" customWidth="1"/>
+    <col min="36" max="36" width="21.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="10.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1704,73 +1707,76 @@
         <v>4</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="O3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="R3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AE3" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AH3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>26</v>
       </c>
-      <c r="AI3" s="8" t="s">
+      <c r="AJ3" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1967</v>
       </c>
@@ -1794,8 +1800,8 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="5"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
@@ -1810,12 +1816,13 @@
       <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
       <c r="AG4" s="4"/>
-      <c r="AH4" s="9">
-        <f>SUM(B4:AG4)</f>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="7">
+        <f>SUM(B4:AH4)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1968</v>
       </c>
@@ -1833,10 +1840,10 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="4">
-        <v>2</v>
-      </c>
-      <c r="O5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4">
+        <v>2</v>
+      </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
@@ -1846,10 +1853,10 @@
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
-      <c r="Y5" s="4">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4">
+        <v>1</v>
+      </c>
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
       <c r="AC5" s="4"/>
@@ -1857,12 +1864,13 @@
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
-      <c r="AH5" s="9">
-        <f t="shared" ref="AH5:AH59" si="0">SUM(B5:AG5)</f>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="7">
+        <f t="shared" ref="AI5:AI58" si="0">SUM(B5:AH5)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1969</v>
       </c>
@@ -1882,17 +1890,17 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4">
+        <v>1</v>
+      </c>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
-      <c r="U6" s="4">
-        <v>2</v>
-      </c>
-      <c r="V6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4">
+        <v>2</v>
+      </c>
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
@@ -1904,12 +1912,13 @@
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
-      <c r="AH6" s="9">
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1970</v>
       </c>
@@ -1927,15 +1936,15 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="4">
+      <c r="N7" s="4"/>
+      <c r="O7" s="4">
         <v>3</v>
       </c>
-      <c r="O7" s="4"/>
       <c r="P7" s="4"/>
-      <c r="Q7" s="4">
-        <v>1</v>
-      </c>
-      <c r="R7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4">
+        <v>1</v>
+      </c>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
@@ -1946,19 +1955,20 @@
       <c r="Z7" s="4"/>
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
-      <c r="AC7" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="4"/>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="4">
+        <v>1</v>
+      </c>
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
       <c r="AG7" s="4"/>
-      <c r="AH7" s="9">
+      <c r="AH7" s="4"/>
+      <c r="AI7" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1971</v>
       </c>
@@ -1976,18 +1986,18 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
-      <c r="N8" s="4">
-        <v>1</v>
-      </c>
-      <c r="O8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4">
+        <v>1</v>
+      </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
-      <c r="T8" s="4">
-        <v>2</v>
-      </c>
-      <c r="U8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4">
+        <v>2</v>
+      </c>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
@@ -1995,19 +2005,20 @@
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
-      <c r="AC8" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD8" s="4"/>
+      <c r="AC8" s="4"/>
+      <c r="AD8" s="4">
+        <v>1</v>
+      </c>
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
       <c r="AG8" s="4"/>
-      <c r="AH8" s="9">
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1972</v>
       </c>
@@ -2031,32 +2042,33 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
-      <c r="T9" s="4">
+      <c r="T9" s="4"/>
+      <c r="U9" s="4">
         <v>3</v>
       </c>
-      <c r="U9" s="4"/>
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
       <c r="Z9" s="4"/>
-      <c r="AA9" s="4">
-        <v>1</v>
-      </c>
-      <c r="AB9" s="4"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4">
+        <v>1</v>
+      </c>
       <c r="AC9" s="4"/>
       <c r="AD9" s="4"/>
       <c r="AE9" s="4"/>
       <c r="AF9" s="4"/>
-      <c r="AG9" s="4">
-        <v>2</v>
-      </c>
-      <c r="AH9" s="9">
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI9" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1973</v>
       </c>
@@ -2077,18 +2089,18 @@
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
-      <c r="Q10" s="4">
-        <v>1</v>
-      </c>
-      <c r="R10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4">
+        <v>1</v>
+      </c>
       <c r="S10" s="4"/>
-      <c r="T10" s="4">
+      <c r="T10" s="4"/>
+      <c r="U10" s="4">
         <v>3</v>
       </c>
-      <c r="U10" s="4">
-        <v>2</v>
-      </c>
-      <c r="V10" s="4"/>
+      <c r="V10" s="4">
+        <v>2</v>
+      </c>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
@@ -2100,12 +2112,13 @@
       <c r="AE10" s="4"/>
       <c r="AF10" s="4"/>
       <c r="AG10" s="4"/>
-      <c r="AH10" s="9">
+      <c r="AH10" s="4"/>
+      <c r="AI10" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>1974</v>
       </c>
@@ -2124,37 +2137,38 @@
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="4">
-        <v>1</v>
-      </c>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4">
-        <v>1</v>
-      </c>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4">
-        <v>2</v>
-      </c>
-      <c r="V11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4">
+        <v>1</v>
+      </c>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4">
+        <v>1</v>
+      </c>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4">
+        <v>2</v>
+      </c>
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
-      <c r="AA11" s="4">
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="4">
         <v>3</v>
       </c>
-      <c r="AB11" s="4"/>
       <c r="AC11" s="4"/>
       <c r="AD11" s="4"/>
       <c r="AE11" s="4"/>
       <c r="AF11" s="4"/>
       <c r="AG11" s="4"/>
-      <c r="AH11" s="9">
+      <c r="AH11" s="4"/>
+      <c r="AI11" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>1975</v>
       </c>
@@ -2175,35 +2189,36 @@
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-      <c r="Q12" s="4">
-        <v>1</v>
-      </c>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4">
-        <v>1</v>
-      </c>
-      <c r="T12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4">
+        <v>1</v>
+      </c>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4">
+        <v>1</v>
+      </c>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
-      <c r="AA12" s="4">
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4">
         <v>3</v>
       </c>
-      <c r="AB12" s="4"/>
       <c r="AC12" s="4"/>
       <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
       <c r="AG12" s="4"/>
-      <c r="AH12" s="9">
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>1976</v>
       </c>
@@ -2222,37 +2237,38 @@
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="4">
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4">
         <v>3</v>
       </c>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4">
-        <v>1</v>
-      </c>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4">
-        <v>2</v>
-      </c>
-      <c r="V13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4">
+        <v>1</v>
+      </c>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4">
+        <v>2</v>
+      </c>
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
       <c r="Z13" s="4"/>
-      <c r="AA13" s="4">
-        <v>1</v>
-      </c>
-      <c r="AB13" s="4"/>
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="4">
+        <v>1</v>
+      </c>
       <c r="AC13" s="4"/>
       <c r="AD13" s="4"/>
       <c r="AE13" s="4"/>
       <c r="AF13" s="4"/>
       <c r="AG13" s="4"/>
-      <c r="AH13" s="9">
+      <c r="AH13" s="4"/>
+      <c r="AI13" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>1977</v>
       </c>
@@ -2275,16 +2291,16 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="4">
-        <v>1</v>
-      </c>
-      <c r="R14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4">
+        <v>1</v>
+      </c>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
-      <c r="U14" s="4">
-        <v>1</v>
-      </c>
-      <c r="V14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4">
+        <v>1</v>
+      </c>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
@@ -2296,12 +2312,13 @@
       <c r="AE14" s="4"/>
       <c r="AF14" s="4"/>
       <c r="AG14" s="4"/>
-      <c r="AH14" s="9">
+      <c r="AH14" s="4"/>
+      <c r="AI14" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>1978</v>
       </c>
@@ -2326,36 +2343,37 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
-      <c r="S15" s="4">
-        <v>1</v>
-      </c>
-      <c r="T15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4">
+        <v>1</v>
+      </c>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
       <c r="Z15" s="4"/>
-      <c r="AA15" s="4">
+      <c r="AA15" s="4"/>
+      <c r="AB15" s="4">
         <v>3</v>
       </c>
-      <c r="AB15" s="4"/>
       <c r="AC15" s="4"/>
       <c r="AD15" s="4"/>
       <c r="AE15" s="4"/>
-      <c r="AF15" s="4">
-        <v>2</v>
-      </c>
-      <c r="AG15" s="4"/>
-      <c r="AH15" s="9">
+      <c r="AF15" s="4"/>
+      <c r="AG15" s="4">
+        <v>2</v>
+      </c>
+      <c r="AH15" s="4"/>
+      <c r="AI15" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AI15" s="8" t="s">
+      <c r="AJ15" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>1979</v>
       </c>
@@ -2376,40 +2394,41 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
-      <c r="S16" s="4">
-        <v>2</v>
-      </c>
-      <c r="T16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4">
+        <v>2</v>
+      </c>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
-      <c r="Z16" s="4">
-        <v>1</v>
-      </c>
+      <c r="Z16" s="4"/>
       <c r="AA16" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="4">
         <v>3</v>
       </c>
-      <c r="AB16" s="4"/>
       <c r="AC16" s="4"/>
       <c r="AD16" s="4"/>
-      <c r="AE16" s="4">
-        <v>1</v>
-      </c>
+      <c r="AE16" s="4"/>
       <c r="AF16" s="4">
-        <v>2</v>
-      </c>
-      <c r="AG16" s="4"/>
-      <c r="AH16" s="9">
+        <v>1</v>
+      </c>
+      <c r="AG16" s="4">
+        <v>2</v>
+      </c>
+      <c r="AH16" s="4"/>
+      <c r="AI16" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AI16" s="8" t="s">
+      <c r="AJ16" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>1980</v>
       </c>
@@ -2430,10 +2449,10 @@
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
-      <c r="Q17" s="4">
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4">
         <v>4</v>
       </c>
-      <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
@@ -2441,27 +2460,28 @@
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
-      <c r="Z17" s="4">
-        <v>2</v>
-      </c>
-      <c r="AA17" s="4"/>
-      <c r="AB17" s="4">
-        <v>1</v>
-      </c>
-      <c r="AC17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4">
+        <v>1</v>
+      </c>
       <c r="AD17" s="4"/>
       <c r="AE17" s="4"/>
       <c r="AF17" s="4"/>
       <c r="AG17" s="4"/>
-      <c r="AH17" s="9">
+      <c r="AH17" s="4"/>
+      <c r="AI17" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AI17" s="8" t="s">
+      <c r="AJ17" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>1981</v>
       </c>
@@ -2487,37 +2507,38 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
-      <c r="R18" s="4">
-        <v>1</v>
-      </c>
-      <c r="S18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4">
+        <v>1</v>
+      </c>
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
-      <c r="X18" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4">
+        <v>1</v>
+      </c>
       <c r="Z18" s="4"/>
       <c r="AA18" s="4"/>
       <c r="AB18" s="4"/>
-      <c r="AC18" s="4">
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4">
         <v>3</v>
       </c>
-      <c r="AD18" s="4"/>
       <c r="AE18" s="4"/>
       <c r="AF18" s="4"/>
       <c r="AG18" s="4"/>
-      <c r="AH18" s="9">
+      <c r="AH18" s="4"/>
+      <c r="AI18" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AI18" s="8" t="s">
+      <c r="AJ18" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>1982</v>
       </c>
@@ -2540,44 +2561,45 @@
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="4">
-        <v>1</v>
-      </c>
+      <c r="Q19" s="4"/>
       <c r="R19" s="4">
         <v>1</v>
       </c>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4">
+      <c r="S19" s="4">
+        <v>1</v>
+      </c>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4">
         <v>3</v>
       </c>
-      <c r="U19" s="4">
-        <v>1</v>
-      </c>
-      <c r="V19" s="4"/>
+      <c r="V19" s="4">
+        <v>1</v>
+      </c>
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
-      <c r="Y19" s="4">
-        <v>2</v>
-      </c>
-      <c r="Z19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4">
+        <v>2</v>
+      </c>
       <c r="AA19" s="4"/>
       <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
       <c r="AD19" s="4"/>
       <c r="AE19" s="4"/>
       <c r="AF19" s="4"/>
-      <c r="AG19" s="4">
+      <c r="AG19" s="4"/>
+      <c r="AH19" s="4">
         <v>4</v>
       </c>
-      <c r="AH19" s="9">
+      <c r="AI19" s="7">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="AI19" s="10" t="s">
+      <c r="AJ19" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>1983</v>
       </c>
@@ -2596,14 +2618,14 @@
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
-      <c r="Q20" s="4">
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4">
         <v>3</v>
       </c>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4">
-        <v>1</v>
-      </c>
-      <c r="T20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4">
+        <v>1</v>
+      </c>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
@@ -2612,26 +2634,27 @@
       <c r="Z20" s="4"/>
       <c r="AA20" s="4"/>
       <c r="AB20" s="4"/>
-      <c r="AC20" s="4">
-        <v>1</v>
-      </c>
+      <c r="AC20" s="4"/>
       <c r="AD20" s="4">
-        <v>2</v>
-      </c>
-      <c r="AE20" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="AE20" s="4">
+        <v>2</v>
+      </c>
       <c r="AF20" s="4"/>
-      <c r="AG20" s="4">
-        <v>2</v>
-      </c>
-      <c r="AH20" s="9">
+      <c r="AG20" s="4"/>
+      <c r="AH20" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI20" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AI20" s="8" t="s">
+      <c r="AJ20" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>1984</v>
       </c>
@@ -2655,39 +2678,40 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
-      <c r="T21" s="4">
-        <v>2</v>
-      </c>
-      <c r="U21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4">
+        <v>2</v>
+      </c>
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
-      <c r="X21" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4">
+        <v>1</v>
+      </c>
       <c r="Z21" s="4"/>
-      <c r="AA21" s="4">
-        <v>1</v>
-      </c>
-      <c r="AB21" s="4"/>
-      <c r="AC21" s="4">
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4">
         <v>3</v>
       </c>
-      <c r="AD21" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE21" s="4"/>
+      <c r="AE21" s="4">
+        <v>1</v>
+      </c>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
-      <c r="AH21" s="9">
+      <c r="AH21" s="4"/>
+      <c r="AI21" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AI21" s="8" t="s">
+      <c r="AJ21" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>1985</v>
       </c>
@@ -2710,21 +2734,21 @@
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
-      <c r="S22" s="4">
-        <v>1</v>
-      </c>
+      <c r="S22" s="4"/>
       <c r="T22" s="4">
         <v>1</v>
       </c>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4">
+      <c r="U22" s="4">
+        <v>1</v>
+      </c>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4">
         <v>3</v>
       </c>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4">
+        <v>1</v>
+      </c>
       <c r="Z22" s="4"/>
       <c r="AA22" s="4"/>
       <c r="AB22" s="4"/>
@@ -2733,15 +2757,16 @@
       <c r="AE22" s="4"/>
       <c r="AF22" s="4"/>
       <c r="AG22" s="4"/>
-      <c r="AH22" s="9">
+      <c r="AH22" s="4"/>
+      <c r="AI22" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AI22" s="8" t="s">
+      <c r="AJ22" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>1986</v>
       </c>
@@ -2771,31 +2796,32 @@
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
       <c r="W23" s="4"/>
-      <c r="X23" s="4">
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4">
         <v>3</v>
       </c>
-      <c r="Y23" s="4">
-        <v>1</v>
-      </c>
-      <c r="Z23" s="4"/>
+      <c r="Z23" s="4">
+        <v>1</v>
+      </c>
       <c r="AA23" s="4"/>
       <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
       <c r="AD23" s="4"/>
       <c r="AE23" s="4"/>
       <c r="AF23" s="4"/>
-      <c r="AG23" s="4">
-        <v>2</v>
-      </c>
-      <c r="AH23" s="9">
+      <c r="AG23" s="4"/>
+      <c r="AH23" s="4">
+        <v>2</v>
+      </c>
+      <c r="AI23" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AI23" s="8" t="s">
+      <c r="AJ23" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>1987</v>
       </c>
@@ -2822,10 +2848,10 @@
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
-      <c r="U24" s="4">
-        <v>2</v>
-      </c>
-      <c r="V24" s="4"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="4">
+        <v>2</v>
+      </c>
       <c r="W24" s="4"/>
       <c r="X24" s="4"/>
       <c r="Y24" s="4"/>
@@ -2835,21 +2861,22 @@
       <c r="AC24" s="4"/>
       <c r="AD24" s="4"/>
       <c r="AE24" s="4"/>
-      <c r="AF24" s="4">
-        <v>1</v>
-      </c>
+      <c r="AF24" s="4"/>
       <c r="AG24" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH24" s="4">
         <v>3</v>
       </c>
-      <c r="AH24" s="9">
+      <c r="AI24" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AI24" s="8" t="s">
+      <c r="AJ24" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>1988</v>
       </c>
@@ -2878,34 +2905,35 @@
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
-      <c r="U25" s="4">
-        <v>1</v>
-      </c>
-      <c r="V25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4">
+        <v>1</v>
+      </c>
       <c r="W25" s="4"/>
       <c r="X25" s="4"/>
       <c r="Y25" s="4"/>
       <c r="Z25" s="4"/>
       <c r="AA25" s="4"/>
       <c r="AB25" s="4"/>
-      <c r="AC25" s="4">
+      <c r="AC25" s="4"/>
+      <c r="AD25" s="4">
         <v>3</v>
       </c>
-      <c r="AD25" s="4"/>
       <c r="AE25" s="4"/>
-      <c r="AF25" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG25" s="4"/>
-      <c r="AH25" s="9">
+      <c r="AF25" s="4"/>
+      <c r="AG25" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH25" s="4"/>
+      <c r="AI25" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AI25" s="8" t="s">
+      <c r="AJ25" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>1989</v>
       </c>
@@ -2930,36 +2958,37 @@
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
-      <c r="S26" s="4">
-        <v>2</v>
-      </c>
-      <c r="T26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4">
+        <v>2</v>
+      </c>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
       <c r="W26" s="4"/>
       <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
       <c r="Z26" s="4"/>
-      <c r="AA26" s="4">
-        <v>1</v>
-      </c>
-      <c r="AB26" s="4"/>
-      <c r="AC26" s="4">
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="4"/>
+      <c r="AD26" s="4">
         <v>3</v>
       </c>
-      <c r="AD26" s="4"/>
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
-      <c r="AH26" s="9">
+      <c r="AH26" s="4"/>
+      <c r="AI26" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AI26" s="8" t="s">
+      <c r="AJ26" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>1990</v>
       </c>
@@ -2984,42 +3013,43 @@
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
-      <c r="Q27" s="4">
-        <v>1</v>
-      </c>
-      <c r="R27" s="11"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4">
-        <v>1</v>
-      </c>
-      <c r="U27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4">
+        <v>1</v>
+      </c>
+      <c r="S27" s="9"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4">
+        <v>1</v>
+      </c>
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
-      <c r="X27" s="4">
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4">
         <v>3</v>
       </c>
-      <c r="Y27" s="4"/>
       <c r="Z27" s="4"/>
       <c r="AA27" s="4"/>
       <c r="AB27" s="4"/>
-      <c r="AC27" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD27" s="4"/>
+      <c r="AC27" s="4"/>
+      <c r="AD27" s="4">
+        <v>1</v>
+      </c>
       <c r="AE27" s="4"/>
       <c r="AF27" s="4"/>
-      <c r="AG27" s="4">
-        <v>1</v>
-      </c>
-      <c r="AH27" s="9">
+      <c r="AG27" s="4"/>
+      <c r="AH27" s="4">
+        <v>1</v>
+      </c>
+      <c r="AI27" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="AI27" s="8" t="s">
+      <c r="AJ27" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>1991</v>
       </c>
@@ -3047,12 +3077,12 @@
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
-      <c r="P28" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="11"/>
-      <c r="S28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4">
+        <v>1</v>
+      </c>
+      <c r="R28" s="4"/>
+      <c r="S28" s="9"/>
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
@@ -3065,21 +3095,22 @@
       <c r="AC28" s="4"/>
       <c r="AD28" s="4"/>
       <c r="AE28" s="4"/>
-      <c r="AF28" s="4">
-        <v>1</v>
-      </c>
+      <c r="AF28" s="4"/>
       <c r="AG28" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH28" s="4">
         <v>3</v>
       </c>
-      <c r="AH28" s="9">
+      <c r="AI28" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="AI28" s="8" t="s">
+      <c r="AJ28" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>1992</v>
       </c>
@@ -3103,41 +3134,42 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
-      <c r="R29" s="11"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4">
-        <v>1</v>
-      </c>
-      <c r="U29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4">
+        <v>1</v>
+      </c>
       <c r="V29" s="4"/>
       <c r="W29" s="4"/>
       <c r="X29" s="4"/>
       <c r="Y29" s="4"/>
-      <c r="Z29" s="4">
-        <v>1</v>
-      </c>
-      <c r="AA29" s="4"/>
-      <c r="AB29" s="4">
-        <v>1</v>
-      </c>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB29" s="4"/>
       <c r="AC29" s="4">
         <v>1</v>
       </c>
-      <c r="AD29" s="4"/>
+      <c r="AD29" s="4">
+        <v>1</v>
+      </c>
       <c r="AE29" s="4"/>
       <c r="AF29" s="4"/>
-      <c r="AG29" s="4">
-        <v>1</v>
-      </c>
-      <c r="AH29" s="9">
+      <c r="AG29" s="4"/>
+      <c r="AH29" s="4">
+        <v>1</v>
+      </c>
+      <c r="AI29" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="AI29" s="8" t="s">
+      <c r="AJ29" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>1993</v>
       </c>
@@ -3161,41 +3193,42 @@
       </c>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
-      <c r="P30" s="4">
-        <v>2</v>
-      </c>
+      <c r="P30" s="4"/>
       <c r="Q30" s="4">
-        <v>1</v>
-      </c>
-      <c r="R30" s="11"/>
-      <c r="S30" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="R30" s="4">
+        <v>1</v>
+      </c>
+      <c r="S30" s="9"/>
       <c r="T30" s="4"/>
       <c r="U30" s="4"/>
       <c r="V30" s="4"/>
       <c r="W30" s="4"/>
-      <c r="X30" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4">
+        <v>1</v>
+      </c>
       <c r="Z30" s="4"/>
       <c r="AA30" s="4"/>
       <c r="AB30" s="4"/>
-      <c r="AC30" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD30" s="4"/>
+      <c r="AC30" s="4"/>
+      <c r="AD30" s="4">
+        <v>1</v>
+      </c>
       <c r="AE30" s="4"/>
       <c r="AF30" s="4"/>
       <c r="AG30" s="4"/>
-      <c r="AH30" s="9">
+      <c r="AH30" s="4"/>
+      <c r="AI30" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="AI30" s="8" t="s">
+      <c r="AJ30" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>1994</v>
       </c>
@@ -3223,39 +3256,40 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
-      <c r="R31" s="11"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4">
-        <v>1</v>
-      </c>
-      <c r="U31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4">
+        <v>1</v>
+      </c>
       <c r="V31" s="4"/>
       <c r="W31" s="4"/>
       <c r="X31" s="4"/>
       <c r="Y31" s="4"/>
       <c r="Z31" s="4"/>
-      <c r="AA31" s="4">
-        <v>1</v>
-      </c>
+      <c r="AA31" s="4"/>
       <c r="AB31" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC31" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD31" s="4">
         <v>3</v>
       </c>
-      <c r="AD31" s="4"/>
       <c r="AE31" s="4"/>
       <c r="AF31" s="4"/>
       <c r="AG31" s="4"/>
-      <c r="AH31" s="9">
+      <c r="AH31" s="4"/>
+      <c r="AI31" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="AI31" s="8" t="s">
+      <c r="AJ31" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>1995</v>
       </c>
@@ -3277,41 +3311,42 @@
       <c r="M32" s="4">
         <v>2</v>
       </c>
-      <c r="N32" s="4">
-        <v>2</v>
-      </c>
-      <c r="O32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4">
+        <v>2</v>
+      </c>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="9"/>
       <c r="T32" s="4"/>
       <c r="U32" s="4"/>
       <c r="V32" s="4"/>
       <c r="W32" s="4"/>
       <c r="X32" s="4"/>
       <c r="Y32" s="4"/>
-      <c r="Z32" s="4">
-        <v>1</v>
-      </c>
+      <c r="Z32" s="4"/>
       <c r="AA32" s="4">
-        <v>2</v>
-      </c>
-      <c r="AB32" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="AB32" s="4">
+        <v>2</v>
+      </c>
       <c r="AC32" s="4"/>
       <c r="AD32" s="4"/>
       <c r="AE32" s="4"/>
       <c r="AF32" s="4"/>
       <c r="AG32" s="4"/>
-      <c r="AH32" s="9">
+      <c r="AH32" s="4"/>
+      <c r="AI32" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="AI32" s="8" t="s">
+      <c r="AJ32" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>1996</v>
       </c>
@@ -3334,42 +3369,43 @@
         <v>3</v>
       </c>
       <c r="N33" s="4"/>
-      <c r="O33" s="4">
-        <v>2</v>
-      </c>
-      <c r="P33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4">
+        <v>2</v>
+      </c>
       <c r="Q33" s="4"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="9"/>
       <c r="T33" s="4"/>
       <c r="U33" s="4"/>
-      <c r="V33" s="4">
-        <v>2</v>
-      </c>
-      <c r="W33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4">
+        <v>2</v>
+      </c>
       <c r="X33" s="4"/>
       <c r="Y33" s="4"/>
       <c r="Z33" s="4"/>
-      <c r="AA33" s="4">
-        <v>1</v>
-      </c>
-      <c r="AB33" s="4"/>
-      <c r="AC33" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD33" s="4"/>
+      <c r="AA33" s="4"/>
+      <c r="AB33" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC33" s="4"/>
+      <c r="AD33" s="4">
+        <v>1</v>
+      </c>
       <c r="AE33" s="4"/>
       <c r="AF33" s="4"/>
       <c r="AG33" s="4"/>
-      <c r="AH33" s="9">
+      <c r="AH33" s="4"/>
+      <c r="AI33" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="AI33" s="8" t="s">
+      <c r="AJ33" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>1997</v>
       </c>
@@ -3393,41 +3429,42 @@
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
-      <c r="R34" s="11"/>
-      <c r="S34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="9"/>
       <c r="T34" s="4"/>
-      <c r="U34" s="4">
-        <v>1</v>
-      </c>
+      <c r="U34" s="4"/>
       <c r="V34" s="4">
         <v>1</v>
       </c>
-      <c r="W34" s="4"/>
+      <c r="W34" s="4">
+        <v>1</v>
+      </c>
       <c r="X34" s="4"/>
       <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>
-      <c r="AA34" s="4">
-        <v>1</v>
-      </c>
-      <c r="AB34" s="4"/>
-      <c r="AC34" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD34" s="4"/>
-      <c r="AE34" s="4">
-        <v>1</v>
-      </c>
-      <c r="AF34" s="4"/>
+      <c r="AA34" s="4"/>
+      <c r="AB34" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="4"/>
+      <c r="AD34" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE34" s="4"/>
+      <c r="AF34" s="4">
+        <v>1</v>
+      </c>
       <c r="AG34" s="4"/>
-      <c r="AH34" s="9">
+      <c r="AH34" s="4"/>
+      <c r="AI34" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="AI34" s="8" t="s">
+      <c r="AJ34" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>1998</v>
       </c>
@@ -3450,44 +3487,45 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
-      <c r="O35" s="4">
-        <v>1</v>
-      </c>
-      <c r="P35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4">
+        <v>1</v>
+      </c>
       <c r="Q35" s="4"/>
-      <c r="R35" s="11"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4">
-        <v>1</v>
-      </c>
+      <c r="R35" s="4"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="4"/>
       <c r="U35" s="4">
         <v>1</v>
       </c>
-      <c r="V35" s="4"/>
+      <c r="V35" s="4">
+        <v>1</v>
+      </c>
       <c r="W35" s="4"/>
       <c r="X35" s="4"/>
-      <c r="Y35" s="4">
-        <v>1</v>
-      </c>
-      <c r="Z35" s="4"/>
+      <c r="Y35" s="4"/>
+      <c r="Z35" s="4">
+        <v>1</v>
+      </c>
       <c r="AA35" s="4"/>
       <c r="AB35" s="4"/>
-      <c r="AC35" s="4">
-        <v>1</v>
-      </c>
-      <c r="AD35" s="4"/>
+      <c r="AC35" s="4"/>
+      <c r="AD35" s="4">
+        <v>1</v>
+      </c>
       <c r="AE35" s="4"/>
       <c r="AF35" s="4"/>
       <c r="AG35" s="4"/>
-      <c r="AH35" s="9">
+      <c r="AH35" s="4"/>
+      <c r="AI35" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="AI35" s="8" t="s">
+      <c r="AJ35" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>1999</v>
       </c>
@@ -3504,22 +3542,22 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
-      <c r="O36" s="4">
-        <v>1</v>
-      </c>
-      <c r="P36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4">
+        <v>1</v>
+      </c>
       <c r="Q36" s="4"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="4">
+      <c r="R36" s="4"/>
+      <c r="S36" s="9"/>
+      <c r="T36" s="4">
         <v>3</v>
       </c>
-      <c r="T36" s="4">
-        <v>1</v>
-      </c>
       <c r="U36" s="4">
         <v>1</v>
       </c>
-      <c r="V36" s="4"/>
+      <c r="V36" s="4">
+        <v>1</v>
+      </c>
       <c r="W36" s="4"/>
       <c r="X36" s="4"/>
       <c r="Y36" s="4"/>
@@ -3528,24 +3566,25 @@
       <c r="AB36" s="4"/>
       <c r="AC36" s="4"/>
       <c r="AD36" s="4"/>
-      <c r="AE36" s="4">
-        <v>1</v>
-      </c>
+      <c r="AE36" s="4"/>
       <c r="AF36" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG36" s="4">
         <v>3</v>
       </c>
-      <c r="AG36" s="4">
-        <v>1</v>
-      </c>
-      <c r="AH36" s="9">
+      <c r="AH36" s="4">
+        <v>1</v>
+      </c>
+      <c r="AI36" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="AI36" s="8" t="s">
+      <c r="AJ36" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>2000</v>
       </c>
@@ -3566,44 +3605,45 @@
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
-      <c r="Q37" s="4">
-        <v>1</v>
-      </c>
-      <c r="R37" s="11"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="4">
-        <v>1</v>
-      </c>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4">
+        <v>1</v>
+      </c>
+      <c r="S37" s="9"/>
+      <c r="T37" s="4"/>
       <c r="U37" s="4">
         <v>1</v>
       </c>
-      <c r="V37" s="4"/>
-      <c r="W37" s="4">
-        <v>1</v>
-      </c>
+      <c r="V37" s="4">
+        <v>1</v>
+      </c>
+      <c r="W37" s="4"/>
       <c r="X37" s="4">
-        <v>2</v>
-      </c>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="4">
-        <v>1</v>
-      </c>
-      <c r="AA37" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="Y37" s="4">
+        <v>2</v>
+      </c>
+      <c r="Z37" s="4"/>
+      <c r="AA37" s="4">
+        <v>1</v>
+      </c>
       <c r="AB37" s="4"/>
       <c r="AC37" s="4"/>
       <c r="AD37" s="4"/>
       <c r="AE37" s="4"/>
       <c r="AF37" s="4"/>
       <c r="AG37" s="4"/>
-      <c r="AH37" s="9">
+      <c r="AH37" s="4"/>
+      <c r="AI37" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="AI37" s="8" t="s">
+      <c r="AJ37" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>2001</v>
       </c>
@@ -3626,1021 +3666,1297 @@
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
-      <c r="Q38" s="4">
-        <v>1</v>
-      </c>
-      <c r="R38" s="11"/>
-      <c r="S38" s="4">
-        <v>2</v>
-      </c>
-      <c r="T38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4">
+        <v>1</v>
+      </c>
+      <c r="S38" s="9"/>
+      <c r="T38" s="4">
+        <v>2</v>
+      </c>
       <c r="U38" s="4"/>
-      <c r="V38" s="4">
+      <c r="V38" s="4"/>
+      <c r="W38" s="4">
         <v>3</v>
       </c>
-      <c r="W38" s="4"/>
       <c r="X38" s="4"/>
       <c r="Y38" s="4"/>
-      <c r="Z38" s="4">
-        <v>2</v>
-      </c>
+      <c r="Z38" s="4"/>
       <c r="AA38" s="4">
-        <v>1</v>
-      </c>
-      <c r="AB38" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="AB38" s="4">
+        <v>1</v>
+      </c>
       <c r="AC38" s="4"/>
       <c r="AD38" s="4"/>
       <c r="AE38" s="4"/>
       <c r="AF38" s="4"/>
       <c r="AG38" s="4"/>
-      <c r="AH38" s="9">
+      <c r="AH38" s="4"/>
+      <c r="AI38" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="AI38" s="8" t="s">
+      <c r="AJ38" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+    <row r="39" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
         <v>2002</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="6"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
-      <c r="W39" s="2"/>
-      <c r="X39" s="2"/>
-      <c r="Y39" s="2"/>
-      <c r="Z39" s="2"/>
-      <c r="AA39" s="2"/>
-      <c r="AB39" s="2"/>
-      <c r="AC39" s="2"/>
-      <c r="AD39" s="2"/>
-      <c r="AE39" s="2"/>
-      <c r="AF39" s="2"/>
-      <c r="AG39" s="2"/>
-      <c r="AH39" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI39" s="8" t="s">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4">
+        <v>1</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4">
+        <v>2</v>
+      </c>
+      <c r="S39" s="9"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="4"/>
+      <c r="Y39" s="4"/>
+      <c r="Z39" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA39" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB39" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC39" s="4"/>
+      <c r="AD39" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE39" s="4"/>
+      <c r="AF39" s="4">
+        <v>3</v>
+      </c>
+      <c r="AG39" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH39" s="4"/>
+      <c r="AI39" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ39" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+    <row r="40" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
         <v>2003</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="6"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="2"/>
-      <c r="U40" s="2"/>
-      <c r="V40" s="2"/>
-      <c r="W40" s="2"/>
-      <c r="X40" s="2"/>
-      <c r="Y40" s="2"/>
-      <c r="Z40" s="2"/>
-      <c r="AA40" s="2"/>
-      <c r="AB40" s="2"/>
-      <c r="AC40" s="2"/>
-      <c r="AD40" s="2"/>
-      <c r="AE40" s="2"/>
-      <c r="AF40" s="2"/>
-      <c r="AG40" s="2"/>
-      <c r="AH40" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI40" s="8" t="s">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4">
+        <v>3</v>
+      </c>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4">
+        <v>1</v>
+      </c>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4">
+        <v>2</v>
+      </c>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="4"/>
+      <c r="U40" s="4"/>
+      <c r="V40" s="4"/>
+      <c r="W40" s="4">
+        <v>3</v>
+      </c>
+      <c r="X40" s="4"/>
+      <c r="Y40" s="4"/>
+      <c r="Z40" s="4"/>
+      <c r="AA40" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB40" s="4"/>
+      <c r="AC40" s="4"/>
+      <c r="AD40" s="4"/>
+      <c r="AE40" s="4"/>
+      <c r="AF40" s="4"/>
+      <c r="AG40" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH40" s="4"/>
+      <c r="AI40" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ40" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+    <row r="41" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
         <v>2004</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
-      <c r="Q41" s="2"/>
-      <c r="R41" s="6"/>
-      <c r="S41" s="2"/>
-      <c r="T41" s="2"/>
-      <c r="U41" s="2"/>
-      <c r="V41" s="2"/>
-      <c r="W41" s="2"/>
-      <c r="X41" s="2"/>
-      <c r="Y41" s="2"/>
-      <c r="Z41" s="2"/>
-      <c r="AA41" s="2"/>
-      <c r="AB41" s="2"/>
-      <c r="AC41" s="2"/>
-      <c r="AD41" s="2"/>
-      <c r="AE41" s="2"/>
-      <c r="AF41" s="2"/>
-      <c r="AG41" s="2"/>
-      <c r="AH41" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI41" s="8" t="s">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4">
+        <v>1</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4">
+        <v>1</v>
+      </c>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="9"/>
+      <c r="T41" s="4">
+        <v>1</v>
+      </c>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4">
+        <v>1</v>
+      </c>
+      <c r="W41" s="4">
+        <v>3</v>
+      </c>
+      <c r="X41" s="4"/>
+      <c r="Y41" s="4"/>
+      <c r="Z41" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA41" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB41" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC41" s="4"/>
+      <c r="AD41" s="4"/>
+      <c r="AE41" s="4"/>
+      <c r="AF41" s="4"/>
+      <c r="AG41" s="4"/>
+      <c r="AH41" s="4"/>
+      <c r="AI41" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ41" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+    <row r="42" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
         <v>2005</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-      <c r="R42" s="6"/>
-      <c r="S42" s="2"/>
-      <c r="T42" s="2"/>
-      <c r="U42" s="2"/>
-      <c r="V42" s="2"/>
-      <c r="W42" s="2"/>
-      <c r="X42" s="2"/>
-      <c r="Y42" s="2"/>
-      <c r="Z42" s="2"/>
-      <c r="AA42" s="2"/>
-      <c r="AB42" s="2"/>
-      <c r="AC42" s="2"/>
-      <c r="AD42" s="2"/>
-      <c r="AE42" s="2"/>
-      <c r="AF42" s="2"/>
-      <c r="AG42" s="2"/>
-      <c r="AH42" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI42" s="8" t="s">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4">
+        <v>2</v>
+      </c>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4">
+        <v>1</v>
+      </c>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="9"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+      <c r="W42" s="4">
+        <v>1</v>
+      </c>
+      <c r="X42" s="4"/>
+      <c r="Y42" s="4"/>
+      <c r="Z42" s="4"/>
+      <c r="AA42" s="4"/>
+      <c r="AB42" s="4">
+        <v>4</v>
+      </c>
+      <c r="AC42" s="4"/>
+      <c r="AD42" s="4"/>
+      <c r="AE42" s="4">
+        <v>2</v>
+      </c>
+      <c r="AF42" s="4"/>
+      <c r="AG42" s="4"/>
+      <c r="AH42" s="4">
+        <v>1</v>
+      </c>
+      <c r="AI42" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ42" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+    <row r="43" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
         <v>2006</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-      <c r="Q43" s="2"/>
-      <c r="R43" s="6"/>
-      <c r="S43" s="2"/>
-      <c r="T43" s="2"/>
-      <c r="U43" s="2"/>
-      <c r="V43" s="2"/>
-      <c r="W43" s="2"/>
-      <c r="X43" s="2"/>
-      <c r="Y43" s="2"/>
-      <c r="Z43" s="2"/>
-      <c r="AA43" s="2"/>
-      <c r="AB43" s="2"/>
-      <c r="AC43" s="2"/>
-      <c r="AD43" s="2"/>
-      <c r="AE43" s="2"/>
-      <c r="AF43" s="2"/>
-      <c r="AG43" s="2"/>
-      <c r="AH43" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI43" s="8" t="s">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4">
+        <v>2</v>
+      </c>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4">
+        <v>4</v>
+      </c>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="9"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+      <c r="W43" s="4">
+        <v>2</v>
+      </c>
+      <c r="X43" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y43" s="4"/>
+      <c r="Z43" s="4"/>
+      <c r="AA43" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB43" s="4"/>
+      <c r="AC43" s="4"/>
+      <c r="AD43" s="4"/>
+      <c r="AE43" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF43" s="4"/>
+      <c r="AG43" s="4"/>
+      <c r="AH43" s="4"/>
+      <c r="AI43" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ43" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+    <row r="44" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
         <v>2007</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
-      <c r="R44" s="6"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="2"/>
-      <c r="U44" s="2"/>
-      <c r="V44" s="2"/>
-      <c r="W44" s="2"/>
-      <c r="X44" s="2"/>
-      <c r="Y44" s="2"/>
-      <c r="Z44" s="2"/>
-      <c r="AA44" s="2"/>
-      <c r="AB44" s="2"/>
-      <c r="AC44" s="2"/>
-      <c r="AD44" s="2"/>
-      <c r="AE44" s="2"/>
-      <c r="AF44" s="2"/>
-      <c r="AG44" s="2"/>
-      <c r="AH44" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI44" s="8" t="s">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4">
+        <v>1</v>
+      </c>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
+      <c r="S44" s="9"/>
+      <c r="T44" s="4"/>
+      <c r="U44" s="4"/>
+      <c r="V44" s="4"/>
+      <c r="W44" s="4">
+        <v>2</v>
+      </c>
+      <c r="X44" s="4"/>
+      <c r="Y44" s="4">
+        <v>4</v>
+      </c>
+      <c r="Z44" s="4"/>
+      <c r="AA44" s="4"/>
+      <c r="AB44" s="4"/>
+      <c r="AC44" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD44" s="4"/>
+      <c r="AE44" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF44" s="4"/>
+      <c r="AG44" s="4"/>
+      <c r="AH44" s="4"/>
+      <c r="AI44" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ44" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+    <row r="45" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
         <v>2008</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-      <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
-      <c r="R45" s="6"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="2"/>
-      <c r="U45" s="2"/>
-      <c r="V45" s="2"/>
-      <c r="W45" s="2"/>
-      <c r="X45" s="2"/>
-      <c r="Y45" s="2"/>
-      <c r="Z45" s="2"/>
-      <c r="AA45" s="2"/>
-      <c r="AB45" s="2"/>
-      <c r="AC45" s="2"/>
-      <c r="AD45" s="2"/>
-      <c r="AE45" s="2"/>
-      <c r="AF45" s="2"/>
-      <c r="AG45" s="2"/>
-      <c r="AH45" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI45" s="8" t="s">
+      <c r="B45" s="4">
+        <v>3</v>
+      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4">
+        <v>2</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="9"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="4"/>
+      <c r="W45" s="4"/>
+      <c r="X45" s="4"/>
+      <c r="Y45" s="4"/>
+      <c r="Z45" s="4"/>
+      <c r="AA45" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB45" s="4">
+        <v>3</v>
+      </c>
+      <c r="AC45" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD45" s="4"/>
+      <c r="AE45" s="4"/>
+      <c r="AF45" s="4"/>
+      <c r="AG45" s="4"/>
+      <c r="AH45" s="4"/>
+      <c r="AI45" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ45" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+    <row r="46" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
         <v>2009</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
-      <c r="R46" s="6"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="2"/>
-      <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
-      <c r="W46" s="2"/>
-      <c r="X46" s="2"/>
-      <c r="Y46" s="2"/>
-      <c r="Z46" s="2"/>
-      <c r="AA46" s="2"/>
-      <c r="AB46" s="2"/>
-      <c r="AC46" s="2"/>
-      <c r="AD46" s="2"/>
-      <c r="AE46" s="2"/>
-      <c r="AF46" s="2"/>
-      <c r="AG46" s="2"/>
-      <c r="AH46" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI46" s="8" t="s">
+      <c r="B46" s="4">
+        <v>1</v>
+      </c>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4">
+        <v>1</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4">
+        <v>1</v>
+      </c>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4">
+        <v>2</v>
+      </c>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="9"/>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4">
+        <v>1</v>
+      </c>
+      <c r="W46" s="4"/>
+      <c r="X46" s="4">
+        <v>3</v>
+      </c>
+      <c r="Y46" s="4"/>
+      <c r="Z46" s="4">
+        <v>2</v>
+      </c>
+      <c r="AA46" s="4"/>
+      <c r="AB46" s="4"/>
+      <c r="AC46" s="4"/>
+      <c r="AD46" s="4"/>
+      <c r="AE46" s="4"/>
+      <c r="AF46" s="4"/>
+      <c r="AG46" s="4"/>
+      <c r="AH46" s="4"/>
+      <c r="AI46" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ46" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+    <row r="47" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
         <v>2010</v>
       </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
-      <c r="Q47" s="2"/>
-      <c r="R47" s="6"/>
-      <c r="S47" s="2"/>
-      <c r="T47" s="2"/>
-      <c r="U47" s="2"/>
-      <c r="V47" s="2"/>
-      <c r="W47" s="2"/>
-      <c r="X47" s="2"/>
-      <c r="Y47" s="2"/>
-      <c r="Z47" s="2"/>
-      <c r="AA47" s="2"/>
-      <c r="AB47" s="2"/>
-      <c r="AC47" s="2"/>
-      <c r="AD47" s="2"/>
-      <c r="AE47" s="2"/>
-      <c r="AF47" s="2"/>
-      <c r="AG47" s="2"/>
-      <c r="AH47" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI47" s="8" t="s">
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4">
+        <v>1</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4">
+        <v>1</v>
+      </c>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4">
+        <v>4</v>
+      </c>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="9"/>
+      <c r="T47" s="4"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+      <c r="W47" s="4"/>
+      <c r="X47" s="4"/>
+      <c r="Y47" s="4"/>
+      <c r="Z47" s="4">
+        <v>2</v>
+      </c>
+      <c r="AA47" s="4"/>
+      <c r="AB47" s="4">
+        <v>2</v>
+      </c>
+      <c r="AC47" s="4"/>
+      <c r="AD47" s="4"/>
+      <c r="AE47" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF47" s="4"/>
+      <c r="AG47" s="4"/>
+      <c r="AH47" s="4"/>
+      <c r="AI47" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ47" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+    <row r="48" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
         <v>2011</v>
       </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-      <c r="R48" s="6"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="2"/>
-      <c r="U48" s="2"/>
-      <c r="V48" s="2"/>
-      <c r="W48" s="2"/>
-      <c r="X48" s="2"/>
-      <c r="Y48" s="2"/>
-      <c r="Z48" s="2"/>
-      <c r="AA48" s="2"/>
-      <c r="AB48" s="2"/>
-      <c r="AC48" s="2"/>
-      <c r="AD48" s="2"/>
-      <c r="AE48" s="2"/>
-      <c r="AF48" s="2"/>
-      <c r="AG48" s="2"/>
-      <c r="AH48" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI48" s="8" t="s">
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4">
+        <v>1</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4">
+        <v>1</v>
+      </c>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4">
+        <v>1</v>
+      </c>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="9"/>
+      <c r="T48" s="4"/>
+      <c r="U48" s="4"/>
+      <c r="V48" s="4"/>
+      <c r="W48" s="4">
+        <v>2</v>
+      </c>
+      <c r="X48" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y48" s="4">
+        <v>4</v>
+      </c>
+      <c r="Z48" s="4"/>
+      <c r="AA48" s="4"/>
+      <c r="AB48" s="4"/>
+      <c r="AC48" s="4"/>
+      <c r="AD48" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE48" s="4"/>
+      <c r="AF48" s="4"/>
+      <c r="AG48" s="4"/>
+      <c r="AH48" s="4"/>
+      <c r="AI48" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ48" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
         <v>2012</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="6"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="2"/>
-      <c r="U49" s="2"/>
-      <c r="V49" s="2"/>
-      <c r="W49" s="2"/>
-      <c r="X49" s="2"/>
-      <c r="Y49" s="2"/>
-      <c r="Z49" s="2"/>
-      <c r="AA49" s="2"/>
-      <c r="AB49" s="2"/>
-      <c r="AC49" s="2"/>
-      <c r="AD49" s="2"/>
-      <c r="AE49" s="2"/>
-      <c r="AF49" s="2"/>
-      <c r="AG49" s="2"/>
-      <c r="AH49" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI49" s="8" t="s">
+      <c r="B49" s="4"/>
+      <c r="C49" s="4">
+        <v>1</v>
+      </c>
+      <c r="D49" s="4">
+        <v>4</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4">
+        <v>1</v>
+      </c>
+      <c r="N49" s="4">
+        <v>1</v>
+      </c>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="9"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="4">
+        <v>1</v>
+      </c>
+      <c r="X49" s="4"/>
+      <c r="Y49" s="4"/>
+      <c r="Z49" s="4"/>
+      <c r="AA49" s="4"/>
+      <c r="AB49" s="4"/>
+      <c r="AC49" s="4"/>
+      <c r="AD49" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE49" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF49" s="4"/>
+      <c r="AG49" s="4"/>
+      <c r="AH49" s="4"/>
+      <c r="AI49" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ49" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
         <v>2013</v>
       </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
-      <c r="Q50" s="2"/>
-      <c r="R50" s="6"/>
-      <c r="S50" s="2"/>
-      <c r="T50" s="2"/>
-      <c r="U50" s="2"/>
-      <c r="V50" s="2"/>
-      <c r="W50" s="2"/>
-      <c r="X50" s="2"/>
-      <c r="Y50" s="2"/>
-      <c r="Z50" s="2"/>
-      <c r="AA50" s="2"/>
-      <c r="AB50" s="2"/>
-      <c r="AC50" s="2"/>
-      <c r="AD50" s="2"/>
-      <c r="AE50" s="2"/>
-      <c r="AF50" s="2"/>
-      <c r="AG50" s="2"/>
-      <c r="AH50" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AI50" s="8" t="s">
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4">
+        <v>2</v>
+      </c>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4">
+        <v>1</v>
+      </c>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="9"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+      <c r="W50" s="4">
+        <v>1</v>
+      </c>
+      <c r="X50" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y50" s="4"/>
+      <c r="Z50" s="4"/>
+      <c r="AA50" s="4"/>
+      <c r="AB50" s="4"/>
+      <c r="AC50" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD50" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE50" s="4">
+        <v>3</v>
+      </c>
+      <c r="AF50" s="4"/>
+      <c r="AG50" s="4"/>
+      <c r="AH50" s="4"/>
+      <c r="AI50" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ50" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
         <v>2014</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-      <c r="O51" s="2"/>
-      <c r="P51" s="2"/>
-      <c r="Q51" s="2"/>
-      <c r="R51" s="6"/>
-      <c r="S51" s="2"/>
-      <c r="T51" s="2"/>
-      <c r="U51" s="2"/>
-      <c r="V51" s="2"/>
-      <c r="W51" s="2"/>
-      <c r="X51" s="2"/>
-      <c r="Y51" s="2"/>
-      <c r="Z51" s="2"/>
-      <c r="AA51" s="2"/>
-      <c r="AB51" s="2"/>
-      <c r="AC51" s="2"/>
-      <c r="AD51" s="2"/>
-      <c r="AE51" s="2"/>
-      <c r="AF51" s="2"/>
-      <c r="AG51" s="2"/>
-      <c r="AH51" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4">
+        <v>1</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4">
+        <v>1</v>
+      </c>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4">
+        <v>1</v>
+      </c>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4">
+        <v>1</v>
+      </c>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4">
+        <v>2</v>
+      </c>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="9"/>
+      <c r="T51" s="4"/>
+      <c r="U51" s="4"/>
+      <c r="V51" s="4"/>
+      <c r="W51" s="4">
+        <v>3</v>
+      </c>
+      <c r="X51" s="4"/>
+      <c r="Y51" s="4"/>
+      <c r="Z51" s="4"/>
+      <c r="AA51" s="4"/>
+      <c r="AB51" s="4"/>
+      <c r="AC51" s="4"/>
+      <c r="AD51" s="4"/>
+      <c r="AE51" s="4">
+        <v>2</v>
+      </c>
+      <c r="AF51" s="4"/>
+      <c r="AG51" s="4"/>
+      <c r="AH51" s="4"/>
+      <c r="AI51" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ51" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
         <v>2015</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-      <c r="O52" s="2"/>
-      <c r="P52" s="2"/>
-      <c r="Q52" s="2"/>
-      <c r="R52" s="2"/>
-      <c r="S52" s="2"/>
-      <c r="T52" s="2"/>
-      <c r="U52" s="2"/>
-      <c r="V52" s="2"/>
-      <c r="W52" s="2"/>
-      <c r="X52" s="2"/>
-      <c r="Y52" s="2"/>
-      <c r="Z52" s="2"/>
-      <c r="AA52" s="2"/>
-      <c r="AB52" s="2"/>
-      <c r="AC52" s="2"/>
-      <c r="AD52" s="2"/>
-      <c r="AE52" s="2"/>
-      <c r="AF52" s="2"/>
-      <c r="AG52" s="2"/>
-      <c r="AH52" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
+      <c r="B52" s="4">
+        <v>1</v>
+      </c>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4">
+        <v>2</v>
+      </c>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4">
+        <v>3</v>
+      </c>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4">
+        <v>1</v>
+      </c>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4">
+        <v>1</v>
+      </c>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+      <c r="U52" s="4"/>
+      <c r="V52" s="4"/>
+      <c r="W52" s="4">
+        <v>1</v>
+      </c>
+      <c r="X52" s="4"/>
+      <c r="Y52" s="4"/>
+      <c r="Z52" s="4"/>
+      <c r="AA52" s="4"/>
+      <c r="AB52" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC52" s="4"/>
+      <c r="AD52" s="4"/>
+      <c r="AE52" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF52" s="4"/>
+      <c r="AG52" s="4"/>
+      <c r="AH52" s="4"/>
+      <c r="AI52" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ52" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
         <v>2016</v>
       </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="O53" s="2"/>
-      <c r="P53" s="2"/>
-      <c r="Q53" s="2"/>
-      <c r="R53" s="7"/>
-      <c r="S53" s="2"/>
-      <c r="T53" s="2"/>
-      <c r="U53" s="2"/>
-      <c r="V53" s="2"/>
-      <c r="W53" s="2"/>
-      <c r="X53" s="2"/>
-      <c r="Y53" s="2"/>
-      <c r="Z53" s="2"/>
-      <c r="AA53" s="2"/>
-      <c r="AB53" s="2"/>
-      <c r="AC53" s="2"/>
-      <c r="AD53" s="2"/>
-      <c r="AE53" s="2"/>
-      <c r="AF53" s="2"/>
-      <c r="AG53" s="2"/>
-      <c r="AH53" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
+      <c r="B53" s="4"/>
+      <c r="C53" s="4">
+        <v>2</v>
+      </c>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4">
+        <v>2</v>
+      </c>
+      <c r="N53" s="4">
+        <v>1</v>
+      </c>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
+      <c r="S53" s="10"/>
+      <c r="T53" s="4"/>
+      <c r="U53" s="4"/>
+      <c r="V53" s="4"/>
+      <c r="W53" s="4">
+        <v>3</v>
+      </c>
+      <c r="X53" s="4"/>
+      <c r="Y53" s="4"/>
+      <c r="Z53" s="4"/>
+      <c r="AA53" s="4"/>
+      <c r="AB53" s="4">
+        <v>2</v>
+      </c>
+      <c r="AC53" s="4"/>
+      <c r="AD53" s="4"/>
+      <c r="AE53" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF53" s="4"/>
+      <c r="AG53" s="4"/>
+      <c r="AH53" s="4"/>
+      <c r="AI53" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ53" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
         <v>2017</v>
       </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
-      <c r="O54" s="2"/>
-      <c r="P54" s="2"/>
-      <c r="Q54" s="2"/>
-      <c r="R54" s="7"/>
-      <c r="S54" s="2"/>
-      <c r="T54" s="2"/>
-      <c r="U54" s="2"/>
-      <c r="V54" s="2"/>
-      <c r="W54" s="2"/>
-      <c r="X54" s="2"/>
-      <c r="Y54" s="2"/>
-      <c r="Z54" s="2"/>
-      <c r="AA54" s="2"/>
-      <c r="AB54" s="2"/>
-      <c r="AC54" s="2"/>
-      <c r="AD54" s="2"/>
-      <c r="AE54" s="2"/>
-      <c r="AF54" s="2"/>
-      <c r="AG54" s="2"/>
-      <c r="AH54" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
+      <c r="B54" s="4"/>
+      <c r="C54" s="4">
+        <v>1</v>
+      </c>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="10"/>
+      <c r="T54" s="4"/>
+      <c r="U54" s="4"/>
+      <c r="V54" s="4">
+        <v>1</v>
+      </c>
+      <c r="W54" s="4">
+        <v>2</v>
+      </c>
+      <c r="X54" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y54" s="4"/>
+      <c r="Z54" s="4"/>
+      <c r="AA54" s="4">
+        <v>3</v>
+      </c>
+      <c r="AB54" s="4"/>
+      <c r="AC54" s="4"/>
+      <c r="AD54" s="4"/>
+      <c r="AE54" s="4"/>
+      <c r="AF54" s="4"/>
+      <c r="AG54" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH54" s="4"/>
+      <c r="AI54" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ54" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
         <v>2018</v>
       </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
-      <c r="O55" s="2"/>
-      <c r="P55" s="2"/>
-      <c r="Q55" s="2"/>
-      <c r="R55" s="7"/>
-      <c r="S55" s="2"/>
-      <c r="T55" s="2"/>
-      <c r="U55" s="2"/>
-      <c r="V55" s="2"/>
-      <c r="W55" s="2"/>
-      <c r="X55" s="2"/>
-      <c r="Y55" s="2"/>
-      <c r="Z55" s="2"/>
-      <c r="AA55" s="2"/>
-      <c r="AB55" s="2"/>
-      <c r="AC55" s="2"/>
-      <c r="AD55" s="2"/>
-      <c r="AE55" s="2"/>
-      <c r="AF55" s="2"/>
-      <c r="AG55" s="2"/>
-      <c r="AH55" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4">
+        <v>1</v>
+      </c>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4">
+        <v>1</v>
+      </c>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4">
+        <v>1</v>
+      </c>
+      <c r="R55" s="4"/>
+      <c r="S55" s="10">
+        <v>1</v>
+      </c>
+      <c r="T55" s="4">
+        <v>2</v>
+      </c>
+      <c r="U55" s="4"/>
+      <c r="V55" s="4"/>
+      <c r="W55" s="4">
+        <v>3</v>
+      </c>
+      <c r="X55" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y55" s="4"/>
+      <c r="Z55" s="4"/>
+      <c r="AA55" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB55" s="4"/>
+      <c r="AC55" s="4"/>
+      <c r="AD55" s="4"/>
+      <c r="AE55" s="4"/>
+      <c r="AF55" s="4"/>
+      <c r="AG55" s="4"/>
+      <c r="AH55" s="4"/>
+      <c r="AI55" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ55" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
         <v>2019</v>
       </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
-      <c r="N56" s="2"/>
-      <c r="O56" s="2"/>
-      <c r="P56" s="2"/>
-      <c r="Q56" s="2"/>
-      <c r="R56" s="7"/>
-      <c r="S56" s="2"/>
-      <c r="T56" s="2"/>
-      <c r="U56" s="2"/>
-      <c r="V56" s="2"/>
-      <c r="W56" s="2"/>
-      <c r="X56" s="2"/>
-      <c r="Y56" s="2"/>
-      <c r="Z56" s="2"/>
-      <c r="AA56" s="2"/>
-      <c r="AB56" s="2"/>
-      <c r="AC56" s="2"/>
-      <c r="AD56" s="2"/>
-      <c r="AE56" s="2"/>
-      <c r="AF56" s="2"/>
-      <c r="AG56" s="2"/>
-      <c r="AH56" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4">
+        <v>1</v>
+      </c>
+      <c r="N56" s="4">
+        <v>1</v>
+      </c>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4">
+        <v>3</v>
+      </c>
+      <c r="R56" s="4"/>
+      <c r="S56" s="10"/>
+      <c r="T56" s="4"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="4">
+        <v>1</v>
+      </c>
+      <c r="W56" s="4"/>
+      <c r="X56" s="4"/>
+      <c r="Y56" s="4"/>
+      <c r="Z56" s="4"/>
+      <c r="AA56" s="4"/>
+      <c r="AB56" s="4"/>
+      <c r="AC56" s="4"/>
+      <c r="AD56" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE56" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF56" s="4"/>
+      <c r="AG56" s="4">
+        <v>2</v>
+      </c>
+      <c r="AH56" s="4"/>
+      <c r="AI56" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="AJ56" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
         <v>2020</v>
       </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
-      <c r="M57" s="2"/>
-      <c r="N57" s="2"/>
-      <c r="O57" s="2"/>
-      <c r="P57" s="2"/>
-      <c r="Q57" s="2"/>
-      <c r="R57" s="7"/>
-      <c r="S57" s="2"/>
-      <c r="T57" s="2"/>
-      <c r="U57" s="2"/>
-      <c r="V57" s="2"/>
-      <c r="W57" s="2"/>
-      <c r="X57" s="2"/>
-      <c r="Y57" s="2"/>
-      <c r="Z57" s="2"/>
-      <c r="AA57" s="2"/>
-      <c r="AB57" s="2"/>
-      <c r="AC57" s="2"/>
-      <c r="AD57" s="2"/>
-      <c r="AE57" s="2"/>
-      <c r="AF57" s="2"/>
-      <c r="AG57" s="2"/>
-      <c r="AH57" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4">
+        <v>1</v>
+      </c>
+      <c r="E57" s="4">
+        <v>2</v>
+      </c>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4">
+        <v>1</v>
+      </c>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4">
+        <v>1</v>
+      </c>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4">
+        <v>2</v>
+      </c>
+      <c r="R57" s="4"/>
+      <c r="S57" s="10"/>
+      <c r="T57" s="4">
+        <v>1</v>
+      </c>
+      <c r="U57" s="4"/>
+      <c r="V57" s="4"/>
+      <c r="W57" s="4"/>
+      <c r="X57" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y57" s="4"/>
+      <c r="Z57" s="4"/>
+      <c r="AA57" s="4"/>
+      <c r="AB57" s="4"/>
+      <c r="AC57" s="4"/>
+      <c r="AD57" s="4"/>
+      <c r="AE57" s="4"/>
+      <c r="AF57" s="4">
+        <v>4</v>
+      </c>
+      <c r="AG57" s="4"/>
+      <c r="AH57" s="4"/>
+      <c r="AI57" s="7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="AJ57" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
         <v>2021</v>
       </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
-      <c r="M58" s="2"/>
-      <c r="N58" s="2"/>
-      <c r="O58" s="2"/>
-      <c r="P58" s="2"/>
-      <c r="Q58" s="2"/>
-      <c r="R58" s="7"/>
-      <c r="S58" s="2"/>
-      <c r="T58" s="2"/>
-      <c r="U58" s="2"/>
-      <c r="V58" s="2"/>
-      <c r="W58" s="2"/>
-      <c r="X58" s="2"/>
-      <c r="Y58" s="2"/>
-      <c r="Z58" s="2"/>
-      <c r="AA58" s="2"/>
-      <c r="AB58" s="2"/>
-      <c r="AC58" s="2"/>
-      <c r="AD58" s="2"/>
-      <c r="AE58" s="2"/>
-      <c r="AF58" s="2"/>
-      <c r="AG58" s="2"/>
-      <c r="AH58" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
-      <c r="O59" s="2"/>
-      <c r="P59" s="2"/>
-      <c r="Q59" s="2"/>
-      <c r="R59" s="7"/>
-      <c r="S59" s="2"/>
-      <c r="T59" s="2"/>
-      <c r="U59" s="2"/>
-      <c r="V59" s="2"/>
-      <c r="W59" s="2"/>
-      <c r="X59" s="2"/>
-      <c r="Y59" s="2"/>
-      <c r="Z59" s="2"/>
-      <c r="AA59" s="2"/>
-      <c r="AB59" s="2"/>
-      <c r="AC59" s="2"/>
-      <c r="AD59" s="2"/>
-      <c r="AE59" s="2"/>
-      <c r="AF59" s="2"/>
-      <c r="AG59" s="2"/>
-      <c r="AH59" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="R60" s="1"/>
-    </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="R61" s="1"/>
-    </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="R62" s="1"/>
-    </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="R63" s="1"/>
-    </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="R64" s="1"/>
-    </row>
-    <row r="65" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R65" s="1"/>
-    </row>
-    <row r="66" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R66" s="1"/>
-    </row>
-    <row r="67" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R67" s="1"/>
-    </row>
-    <row r="68" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R68" s="1"/>
-    </row>
-    <row r="69" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R69" s="1"/>
-    </row>
-    <row r="70" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R70" s="1"/>
-    </row>
-    <row r="71" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R71" s="1"/>
-    </row>
-    <row r="72" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R72" s="1"/>
-    </row>
-    <row r="73" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R73" s="1"/>
-    </row>
-    <row r="74" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R74" s="1"/>
-    </row>
-    <row r="75" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R75" s="1"/>
-    </row>
-    <row r="76" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R76" s="1"/>
-    </row>
-    <row r="77" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R77" s="1"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4">
+        <v>1</v>
+      </c>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4">
+        <v>3</v>
+      </c>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4">
+        <v>2</v>
+      </c>
+      <c r="R58" s="4"/>
+      <c r="S58" s="10"/>
+      <c r="T58" s="4">
+        <v>4</v>
+      </c>
+      <c r="U58" s="4"/>
+      <c r="V58" s="4"/>
+      <c r="W58" s="4"/>
+      <c r="X58" s="4"/>
+      <c r="Y58" s="4"/>
+      <c r="Z58" s="4"/>
+      <c r="AA58" s="4"/>
+      <c r="AB58" s="4"/>
+      <c r="AC58" s="4"/>
+      <c r="AD58" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE58" s="4"/>
+      <c r="AF58" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG58" s="4"/>
+      <c r="AH58" s="4"/>
+      <c r="AI58" s="7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="AJ58" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="S59" s="1"/>
+    </row>
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="S60" s="1"/>
+    </row>
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="S61" s="1"/>
+    </row>
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="S62" s="1"/>
+    </row>
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="S63" s="1"/>
+    </row>
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="S64" s="1"/>
+    </row>
+    <row r="65" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S65" s="1"/>
+    </row>
+    <row r="66" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S66" s="1"/>
+    </row>
+    <row r="67" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S67" s="1"/>
+    </row>
+    <row r="68" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S68" s="1"/>
+    </row>
+    <row r="69" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S69" s="1"/>
+    </row>
+    <row r="70" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S70" s="1"/>
+    </row>
+    <row r="71" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S71" s="1"/>
+    </row>
+    <row r="72" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S72" s="1"/>
+    </row>
+    <row r="73" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S73" s="1"/>
+    </row>
+    <row r="74" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S74" s="1"/>
+    </row>
+    <row r="75" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S75" s="1"/>
+    </row>
+    <row r="76" spans="19:19" x14ac:dyDescent="0.25">
+      <c r="S76" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="R1:R76">
-    <sortCondition ref="R1"/>
+  <sortState ref="S1:S76">
+    <sortCondition ref="S1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="Q3" r:id="rId1" display="https://www.nfl.com/teams/las-vegas-raiders/"/>
-    <hyperlink ref="N3" r:id="rId2" display="https://www.nfl.com/teams/indianapolis-colts/"/>
-    <hyperlink ref="S3" r:id="rId3" display="https://www.nfl.com/teams/los-angeles-rams/"/>
+    <hyperlink ref="R3" r:id="rId1" display="https://www.nfl.com/teams/las-vegas-raiders/"/>
+    <hyperlink ref="O3" r:id="rId2" display="https://www.nfl.com/teams/indianapolis-colts/"/>
+    <hyperlink ref="T3" r:id="rId3" display="https://www.nfl.com/teams/los-angeles-rams/"/>
     <hyperlink ref="M3" r:id="rId4" display="https://www.nfl.com/teams/green-bay-packers/"/>
-    <hyperlink ref="AF3" r:id="rId5" display="https://www.nfl.com/teams/tennessee-titans/"/>
+    <hyperlink ref="AG3" r:id="rId5" display="https://www.nfl.com/teams/tennessee-titans/"/>
     <hyperlink ref="I3" r:id="rId6" display="https://www.nfl.com/teams/cleveland-browns/"/>
     <hyperlink ref="J3" r:id="rId7" display="https://www.nfl.com/teams/dallas-cowboys/"/>
-    <hyperlink ref="P3" r:id="rId8" display="https://www.nfl.com/teams/kansas-city-chiefs/"/>
-    <hyperlink ref="R3" r:id="rId9" display="https://www.nfl.com/teams/los-angeles-chargers/"/>
-    <hyperlink ref="Y3" r:id="rId10" display="https://www.nfl.com/teams/new-york-jets/"/>
+    <hyperlink ref="Q3" r:id="rId8" display="https://www.nfl.com/teams/kansas-city-chiefs/"/>
+    <hyperlink ref="S3" r:id="rId9" display="https://www.nfl.com/teams/los-angeles-chargers/"/>
+    <hyperlink ref="Z3" r:id="rId10" display="https://www.nfl.com/teams/new-york-jets/"/>
     <hyperlink ref="G3" r:id="rId11" display="https://www.nfl.com/teams/chicago-bears/"/>
-    <hyperlink ref="X3" r:id="rId12" display="https://www.nfl.com/teams/new-york-giants/"/>
-    <hyperlink ref="AC3" r:id="rId13" display="https://www.nfl.com/teams/san-francisco-49ers/"/>
+    <hyperlink ref="Y3" r:id="rId12" display="https://www.nfl.com/teams/new-york-giants/"/>
+    <hyperlink ref="AD3" r:id="rId13" display="https://www.nfl.com/teams/san-francisco-49ers/"/>
     <hyperlink ref="B3" r:id="rId14" display="https://www.nfl.com/teams/arizona-cardinals/"/>
-    <hyperlink ref="Z3" r:id="rId15" display="https://www.nfl.com/teams/philadelphia-eagles/"/>
-    <hyperlink ref="AG3" r:id="rId16" display="https://www.nfl.com/teams/washington-commanders/"/>
+    <hyperlink ref="AA3" r:id="rId15" display="https://www.nfl.com/teams/philadelphia-eagles/"/>
+    <hyperlink ref="AH3" r:id="rId16" display="https://www.nfl.com/teams/washington-commanders/"/>
     <hyperlink ref="L3" r:id="rId17" display="https://www.nfl.com/teams/detroit-lions/"/>
-    <hyperlink ref="AA3" r:id="rId18" display="https://www.nfl.com/teams/pittsburgh-steelers/"/>
+    <hyperlink ref="AB3" r:id="rId18" display="https://www.nfl.com/teams/pittsburgh-steelers/"/>
     <hyperlink ref="E3" r:id="rId19" display="https://www.nfl.com/teams/buffalo-bills/"/>
-    <hyperlink ref="T3" r:id="rId20" display="https://www.nfl.com/teams/miami-dolphins/"/>
-    <hyperlink ref="U3" r:id="rId21" display="https://www.nfl.com/teams/minnesota-vikings/"/>
-    <hyperlink ref="V3" r:id="rId22" display="https://www.nfl.com/teams/new-england-patriots/"/>
+    <hyperlink ref="U3" r:id="rId20" display="https://www.nfl.com/teams/miami-dolphins/"/>
+    <hyperlink ref="V3" r:id="rId21" display="https://www.nfl.com/teams/minnesota-vikings/"/>
+    <hyperlink ref="W3" r:id="rId22" display="https://www.nfl.com/teams/new-england-patriots/"/>
     <hyperlink ref="K3" r:id="rId23" display="https://www.nfl.com/teams/denver-broncos/"/>
-    <hyperlink ref="W3" r:id="rId24" display="https://www.nfl.com/teams/new-orleans-saints/"/>
+    <hyperlink ref="X3" r:id="rId24" display="https://www.nfl.com/teams/new-orleans-saints/"/>
     <hyperlink ref="C3" r:id="rId25" display="https://www.nfl.com/teams/atlanta-falcons/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>